<commit_message>
Ajuste de nombres de metodos y parametros
-Se ajustaron muchos nombres de metodos y sus tipos de parametros de
entrada para que tengan más sentido y sean más útiles.
-Se añadió un componente temporal que proporciona botones útiles para
depurar bugs en partidas.
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -549,33 +549,6 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,6 +596,33 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -632,15 +632,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -650,6 +641,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,7 +973,7 @@
   <dimension ref="A1:AR51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Z22" sqref="Z22:AA23"/>
+      <selection activeCell="V19" sqref="V19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,46 +988,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
-      <c r="AA1" s="11"/>
-      <c r="AB1" s="11"/>
-      <c r="AC1" s="11"/>
-      <c r="AD1" s="11"/>
-      <c r="AE1" s="11"/>
-      <c r="AF1" s="11"/>
-      <c r="AG1" s="11"/>
-      <c r="AH1" s="11"/>
-      <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -1036,44 +1036,44 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="11"/>
-      <c r="M2" s="11"/>
-      <c r="N2" s="11"/>
-      <c r="O2" s="11"/>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11"/>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="11"/>
-      <c r="V2" s="11"/>
-      <c r="W2" s="11"/>
-      <c r="X2" s="11"/>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="11"/>
-      <c r="AB2" s="11"/>
-      <c r="AC2" s="11"/>
-      <c r="AD2" s="11"/>
-      <c r="AE2" s="11"/>
-      <c r="AF2" s="11"/>
-      <c r="AG2" s="11"/>
-      <c r="AH2" s="11"/>
-      <c r="AI2" s="11"/>
-      <c r="AJ2" s="11"/>
-      <c r="AK2" s="11"/>
-      <c r="AL2" s="11"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
@@ -1082,52 +1082,52 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="15"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="40"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
@@ -1136,48 +1136,48 @@
       <c r="AR3" s="1"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="16"/>
-      <c r="B4" s="17"/>
-      <c r="C4" s="17"/>
-      <c r="D4" s="18" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="18"/>
-      <c r="N4" s="18"/>
-      <c r="O4" s="18"/>
-      <c r="P4" s="18"/>
-      <c r="Q4" s="18"/>
-      <c r="R4" s="18"/>
-      <c r="S4" s="18" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="18"/>
-      <c r="U4" s="18"/>
-      <c r="V4" s="18"/>
-      <c r="W4" s="18"/>
-      <c r="X4" s="18"/>
-      <c r="Y4" s="18"/>
-      <c r="Z4" s="18"/>
-      <c r="AA4" s="18"/>
-      <c r="AB4" s="18"/>
-      <c r="AC4" s="18"/>
-      <c r="AD4" s="18"/>
-      <c r="AE4" s="18"/>
-      <c r="AF4" s="18"/>
-      <c r="AG4" s="18"/>
-      <c r="AH4" s="18"/>
-      <c r="AI4" s="18"/>
-      <c r="AJ4" s="18"/>
-      <c r="AK4" s="18"/>
-      <c r="AL4" s="19"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
+      <c r="AG4" s="43"/>
+      <c r="AH4" s="43"/>
+      <c r="AI4" s="43"/>
+      <c r="AJ4" s="43"/>
+      <c r="AK4" s="43"/>
+      <c r="AL4" s="44"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
@@ -1186,112 +1186,112 @@
       <c r="AR4" s="1"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
-      <c r="B5" s="17"/>
-      <c r="C5" s="17"/>
-      <c r="D5" s="20">
+      <c r="A5" s="37"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="11">
         <v>17</v>
       </c>
-      <c r="E5" s="20">
+      <c r="E5" s="11">
         <v>18</v>
       </c>
-      <c r="F5" s="20">
+      <c r="F5" s="11">
         <v>19</v>
       </c>
-      <c r="G5" s="20">
+      <c r="G5" s="11">
         <v>20</v>
       </c>
-      <c r="H5" s="20">
+      <c r="H5" s="11">
         <v>21</v>
       </c>
-      <c r="I5" s="20">
+      <c r="I5" s="11">
         <v>22</v>
       </c>
-      <c r="J5" s="20">
+      <c r="J5" s="11">
         <v>23</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="11">
         <v>24</v>
       </c>
-      <c r="L5" s="20">
+      <c r="L5" s="11">
         <v>25</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="11">
         <v>26</v>
       </c>
-      <c r="N5" s="20">
+      <c r="N5" s="11">
         <v>27</v>
       </c>
-      <c r="O5" s="20">
+      <c r="O5" s="11">
         <v>28</v>
       </c>
-      <c r="P5" s="20">
+      <c r="P5" s="11">
         <v>29</v>
       </c>
-      <c r="Q5" s="20">
+      <c r="Q5" s="11">
         <v>30</v>
       </c>
-      <c r="R5" s="20">
+      <c r="R5" s="11">
         <v>31</v>
       </c>
-      <c r="S5" s="20">
+      <c r="S5" s="11">
         <v>1</v>
       </c>
-      <c r="T5" s="20">
+      <c r="T5" s="11">
         <v>2</v>
       </c>
-      <c r="U5" s="20">
+      <c r="U5" s="11">
         <v>3</v>
       </c>
-      <c r="V5" s="20">
+      <c r="V5" s="11">
         <v>4</v>
       </c>
-      <c r="W5" s="20">
+      <c r="W5" s="11">
         <v>5</v>
       </c>
-      <c r="X5" s="20">
+      <c r="X5" s="11">
         <v>6</v>
       </c>
-      <c r="Y5" s="20">
+      <c r="Y5" s="11">
         <v>7</v>
       </c>
-      <c r="Z5" s="20">
+      <c r="Z5" s="11">
         <v>8</v>
       </c>
-      <c r="AA5" s="20">
+      <c r="AA5" s="11">
         <v>9</v>
       </c>
-      <c r="AB5" s="20">
+      <c r="AB5" s="11">
         <v>10</v>
       </c>
-      <c r="AC5" s="20">
+      <c r="AC5" s="11">
         <v>11</v>
       </c>
-      <c r="AD5" s="20">
+      <c r="AD5" s="11">
         <v>12</v>
       </c>
-      <c r="AE5" s="20">
+      <c r="AE5" s="11">
         <v>13</v>
       </c>
-      <c r="AF5" s="20">
+      <c r="AF5" s="11">
         <v>14</v>
       </c>
-      <c r="AG5" s="20">
+      <c r="AG5" s="11">
         <v>15</v>
       </c>
-      <c r="AH5" s="20">
+      <c r="AH5" s="11">
         <v>16</v>
       </c>
-      <c r="AI5" s="20">
+      <c r="AI5" s="11">
         <v>17</v>
       </c>
-      <c r="AJ5" s="20">
+      <c r="AJ5" s="11">
         <v>18</v>
       </c>
-      <c r="AK5" s="20">
+      <c r="AK5" s="11">
         <v>19</v>
       </c>
-      <c r="AL5" s="21">
+      <c r="AL5" s="12">
         <v>20</v>
       </c>
       <c r="AM5" s="1"/>
@@ -1302,50 +1302,50 @@
       <c r="AR5" s="1"/>
     </row>
     <row r="6" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A6" s="22">
+      <c r="A6" s="13">
         <v>1</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="26"/>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="27"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="27"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="27"/>
-      <c r="S6" s="27"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="27"/>
-      <c r="X6" s="27"/>
-      <c r="Y6" s="27"/>
-      <c r="Z6" s="27"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="27"/>
-      <c r="AC6" s="27"/>
-      <c r="AD6" s="27"/>
-      <c r="AE6" s="27"/>
-      <c r="AF6" s="27"/>
-      <c r="AG6" s="27"/>
-      <c r="AH6" s="27"/>
-      <c r="AI6" s="27"/>
-      <c r="AJ6" s="27"/>
-      <c r="AK6" s="27"/>
-      <c r="AL6" s="28"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="18"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="18"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="18"/>
+      <c r="T6" s="18"/>
+      <c r="U6" s="18"/>
+      <c r="V6" s="18"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="18"/>
+      <c r="Y6" s="18"/>
+      <c r="Z6" s="18"/>
+      <c r="AA6" s="18"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="18"/>
+      <c r="AD6" s="18"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="18"/>
+      <c r="AG6" s="18"/>
+      <c r="AH6" s="18"/>
+      <c r="AI6" s="18"/>
+      <c r="AJ6" s="18"/>
+      <c r="AK6" s="18"/>
+      <c r="AL6" s="19"/>
       <c r="AM6" s="1"/>
       <c r="AN6" s="1"/>
       <c r="AO6" s="1"/>
@@ -1354,50 +1354,50 @@
       <c r="AR6" s="1"/>
     </row>
     <row r="7" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A7" s="29">
+      <c r="A7" s="20">
         <v>2</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="31"/>
-      <c r="E7" s="31"/>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
-      <c r="K7" s="27"/>
-      <c r="L7" s="27"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="27"/>
-      <c r="Q7" s="27"/>
-      <c r="R7" s="27"/>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
-      <c r="U7" s="27"/>
-      <c r="V7" s="27"/>
-      <c r="W7" s="27"/>
-      <c r="X7" s="27"/>
-      <c r="Y7" s="27"/>
-      <c r="Z7" s="27"/>
-      <c r="AA7" s="27"/>
-      <c r="AB7" s="27"/>
-      <c r="AC7" s="27"/>
-      <c r="AD7" s="27"/>
-      <c r="AE7" s="27"/>
-      <c r="AF7" s="27"/>
-      <c r="AG7" s="27"/>
-      <c r="AH7" s="27"/>
-      <c r="AI7" s="27"/>
-      <c r="AJ7" s="27"/>
-      <c r="AK7" s="27"/>
-      <c r="AL7" s="28"/>
+      <c r="D7" s="22"/>
+      <c r="E7" s="22"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="18"/>
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="18"/>
+      <c r="O7" s="18"/>
+      <c r="P7" s="18"/>
+      <c r="Q7" s="18"/>
+      <c r="R7" s="18"/>
+      <c r="S7" s="18"/>
+      <c r="T7" s="18"/>
+      <c r="U7" s="18"/>
+      <c r="V7" s="18"/>
+      <c r="W7" s="18"/>
+      <c r="X7" s="18"/>
+      <c r="Y7" s="18"/>
+      <c r="Z7" s="18"/>
+      <c r="AA7" s="18"/>
+      <c r="AB7" s="18"/>
+      <c r="AC7" s="18"/>
+      <c r="AD7" s="18"/>
+      <c r="AE7" s="18"/>
+      <c r="AF7" s="18"/>
+      <c r="AG7" s="18"/>
+      <c r="AH7" s="18"/>
+      <c r="AI7" s="18"/>
+      <c r="AJ7" s="18"/>
+      <c r="AK7" s="18"/>
+      <c r="AL7" s="19"/>
       <c r="AM7" s="1"/>
       <c r="AN7" s="1"/>
       <c r="AO7" s="1"/>
@@ -1406,50 +1406,50 @@
       <c r="AR7" s="1"/>
     </row>
     <row r="8" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A8" s="22">
+      <c r="A8" s="13">
         <v>3</v>
       </c>
-      <c r="B8" s="34" t="s">
+      <c r="B8" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="26"/>
-      <c r="I8" s="27"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="27"/>
-      <c r="L8" s="27"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="27"/>
-      <c r="P8" s="27"/>
-      <c r="Q8" s="27"/>
-      <c r="R8" s="27"/>
-      <c r="S8" s="27"/>
-      <c r="T8" s="27"/>
-      <c r="U8" s="27"/>
-      <c r="V8" s="27"/>
-      <c r="W8" s="27"/>
-      <c r="X8" s="27"/>
-      <c r="Y8" s="27"/>
-      <c r="Z8" s="27"/>
-      <c r="AA8" s="27"/>
-      <c r="AB8" s="27"/>
-      <c r="AC8" s="27"/>
-      <c r="AD8" s="27"/>
-      <c r="AE8" s="27"/>
-      <c r="AF8" s="27"/>
-      <c r="AG8" s="27"/>
-      <c r="AH8" s="27"/>
-      <c r="AI8" s="27"/>
-      <c r="AJ8" s="27"/>
-      <c r="AK8" s="27"/>
-      <c r="AL8" s="28"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="18"/>
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="18"/>
+      <c r="O8" s="18"/>
+      <c r="P8" s="18"/>
+      <c r="Q8" s="18"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="18"/>
+      <c r="T8" s="18"/>
+      <c r="U8" s="18"/>
+      <c r="V8" s="18"/>
+      <c r="W8" s="18"/>
+      <c r="X8" s="18"/>
+      <c r="Y8" s="18"/>
+      <c r="Z8" s="18"/>
+      <c r="AA8" s="18"/>
+      <c r="AB8" s="18"/>
+      <c r="AC8" s="18"/>
+      <c r="AD8" s="18"/>
+      <c r="AE8" s="18"/>
+      <c r="AF8" s="18"/>
+      <c r="AG8" s="18"/>
+      <c r="AH8" s="18"/>
+      <c r="AI8" s="18"/>
+      <c r="AJ8" s="18"/>
+      <c r="AK8" s="18"/>
+      <c r="AL8" s="19"/>
       <c r="AM8" s="1"/>
       <c r="AN8" s="1"/>
       <c r="AO8" s="1"/>
@@ -1458,50 +1458,50 @@
       <c r="AR8" s="1"/>
     </row>
     <row r="9" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A9" s="22">
+      <c r="A9" s="13">
         <v>4</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="26"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
-      <c r="I9" s="27"/>
-      <c r="J9" s="27"/>
-      <c r="K9" s="27"/>
-      <c r="L9" s="27"/>
-      <c r="M9" s="27"/>
-      <c r="N9" s="27"/>
-      <c r="O9" s="27"/>
-      <c r="P9" s="27"/>
-      <c r="Q9" s="27"/>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="T9" s="27"/>
-      <c r="U9" s="27"/>
-      <c r="V9" s="27"/>
-      <c r="W9" s="27"/>
-      <c r="X9" s="27"/>
-      <c r="Y9" s="27"/>
-      <c r="Z9" s="27"/>
-      <c r="AA9" s="27"/>
-      <c r="AB9" s="27"/>
-      <c r="AC9" s="27"/>
-      <c r="AD9" s="27"/>
-      <c r="AE9" s="27"/>
-      <c r="AF9" s="27"/>
-      <c r="AG9" s="27"/>
-      <c r="AH9" s="27"/>
-      <c r="AI9" s="27"/>
-      <c r="AJ9" s="27"/>
-      <c r="AK9" s="27"/>
-      <c r="AL9" s="28"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="18"/>
+      <c r="J9" s="18"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="18"/>
+      <c r="P9" s="18"/>
+      <c r="Q9" s="18"/>
+      <c r="R9" s="18"/>
+      <c r="S9" s="18"/>
+      <c r="T9" s="18"/>
+      <c r="U9" s="18"/>
+      <c r="V9" s="18"/>
+      <c r="W9" s="18"/>
+      <c r="X9" s="18"/>
+      <c r="Y9" s="18"/>
+      <c r="Z9" s="18"/>
+      <c r="AA9" s="18"/>
+      <c r="AB9" s="18"/>
+      <c r="AC9" s="18"/>
+      <c r="AD9" s="18"/>
+      <c r="AE9" s="18"/>
+      <c r="AF9" s="18"/>
+      <c r="AG9" s="18"/>
+      <c r="AH9" s="18"/>
+      <c r="AI9" s="18"/>
+      <c r="AJ9" s="18"/>
+      <c r="AK9" s="18"/>
+      <c r="AL9" s="19"/>
       <c r="AM9" s="1"/>
       <c r="AN9" s="1"/>
       <c r="AO9" s="1"/>
@@ -1510,50 +1510,50 @@
       <c r="AR9" s="1"/>
     </row>
     <row r="10" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A10" s="29">
+      <c r="A10" s="20">
         <v>5</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="15" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="26"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
-      <c r="I10" s="26"/>
-      <c r="J10" s="26"/>
-      <c r="K10" s="26"/>
-      <c r="L10" s="26"/>
-      <c r="M10" s="26"/>
-      <c r="N10" s="26"/>
-      <c r="O10" s="26"/>
-      <c r="P10" s="26"/>
-      <c r="Q10" s="26"/>
-      <c r="R10" s="27"/>
-      <c r="S10" s="27"/>
-      <c r="T10" s="27"/>
-      <c r="U10" s="27"/>
-      <c r="V10" s="27"/>
-      <c r="W10" s="27"/>
-      <c r="X10" s="27"/>
-      <c r="Y10" s="27"/>
-      <c r="Z10" s="27"/>
-      <c r="AA10" s="27"/>
-      <c r="AB10" s="27"/>
-      <c r="AC10" s="27"/>
-      <c r="AD10" s="27"/>
-      <c r="AE10" s="27"/>
-      <c r="AF10" s="27"/>
-      <c r="AG10" s="27"/>
-      <c r="AH10" s="27"/>
-      <c r="AI10" s="27"/>
-      <c r="AJ10" s="27"/>
-      <c r="AK10" s="27"/>
-      <c r="AL10" s="28"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="H10" s="17"/>
+      <c r="I10" s="17"/>
+      <c r="J10" s="17"/>
+      <c r="K10" s="17"/>
+      <c r="L10" s="17"/>
+      <c r="M10" s="17"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="17"/>
+      <c r="P10" s="17"/>
+      <c r="Q10" s="17"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
+      <c r="AB10" s="18"/>
+      <c r="AC10" s="18"/>
+      <c r="AD10" s="18"/>
+      <c r="AE10" s="18"/>
+      <c r="AF10" s="18"/>
+      <c r="AG10" s="18"/>
+      <c r="AH10" s="18"/>
+      <c r="AI10" s="18"/>
+      <c r="AJ10" s="18"/>
+      <c r="AK10" s="18"/>
+      <c r="AL10" s="19"/>
       <c r="AM10" s="1"/>
       <c r="AN10" s="1"/>
       <c r="AO10" s="1"/>
@@ -1562,50 +1562,50 @@
       <c r="AR10" s="1"/>
     </row>
     <row r="11" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A11" s="22">
+      <c r="A11" s="13">
         <v>6</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="D11" s="26"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="26"/>
-      <c r="Q11" s="26"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="27"/>
-      <c r="T11" s="27"/>
-      <c r="U11" s="27"/>
-      <c r="V11" s="27"/>
-      <c r="W11" s="27"/>
-      <c r="X11" s="27"/>
-      <c r="Y11" s="27"/>
-      <c r="Z11" s="27"/>
-      <c r="AA11" s="27"/>
-      <c r="AB11" s="27"/>
-      <c r="AC11" s="27"/>
-      <c r="AD11" s="27"/>
-      <c r="AE11" s="27"/>
-      <c r="AF11" s="27"/>
-      <c r="AG11" s="27"/>
-      <c r="AH11" s="27"/>
-      <c r="AI11" s="27"/>
-      <c r="AJ11" s="27"/>
-      <c r="AK11" s="27"/>
-      <c r="AL11" s="28"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="16"/>
+      <c r="H11" s="17"/>
+      <c r="I11" s="17"/>
+      <c r="J11" s="17"/>
+      <c r="K11" s="17"/>
+      <c r="L11" s="17"/>
+      <c r="M11" s="17"/>
+      <c r="N11" s="17"/>
+      <c r="O11" s="17"/>
+      <c r="P11" s="17"/>
+      <c r="Q11" s="17"/>
+      <c r="R11" s="18"/>
+      <c r="S11" s="18"/>
+      <c r="T11" s="18"/>
+      <c r="U11" s="18"/>
+      <c r="V11" s="18"/>
+      <c r="W11" s="18"/>
+      <c r="X11" s="18"/>
+      <c r="Y11" s="18"/>
+      <c r="Z11" s="18"/>
+      <c r="AA11" s="18"/>
+      <c r="AB11" s="18"/>
+      <c r="AC11" s="18"/>
+      <c r="AD11" s="18"/>
+      <c r="AE11" s="18"/>
+      <c r="AF11" s="18"/>
+      <c r="AG11" s="18"/>
+      <c r="AH11" s="18"/>
+      <c r="AI11" s="18"/>
+      <c r="AJ11" s="18"/>
+      <c r="AK11" s="18"/>
+      <c r="AL11" s="19"/>
       <c r="AM11" s="1"/>
       <c r="AN11" s="1"/>
       <c r="AO11" s="1"/>
@@ -1614,50 +1614,50 @@
       <c r="AR11" s="1"/>
     </row>
     <row r="12" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A12" s="22">
+      <c r="A12" s="13">
         <v>7</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="27"/>
-      <c r="L12" s="27"/>
-      <c r="M12" s="27"/>
-      <c r="N12" s="27"/>
-      <c r="O12" s="27"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="27"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="27"/>
-      <c r="X12" s="27"/>
-      <c r="Y12" s="27"/>
-      <c r="Z12" s="27"/>
-      <c r="AA12" s="27"/>
-      <c r="AB12" s="27"/>
-      <c r="AC12" s="27"/>
-      <c r="AD12" s="27"/>
-      <c r="AE12" s="27"/>
-      <c r="AF12" s="27"/>
-      <c r="AG12" s="27"/>
-      <c r="AH12" s="27"/>
-      <c r="AI12" s="27"/>
-      <c r="AJ12" s="27"/>
-      <c r="AK12" s="27"/>
-      <c r="AL12" s="28"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="18"/>
+      <c r="G12" s="18"/>
+      <c r="H12" s="22"/>
+      <c r="I12" s="22"/>
+      <c r="J12" s="17"/>
+      <c r="K12" s="18"/>
+      <c r="L12" s="18"/>
+      <c r="M12" s="18"/>
+      <c r="N12" s="18"/>
+      <c r="O12" s="18"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="18"/>
+      <c r="R12" s="18"/>
+      <c r="S12" s="18"/>
+      <c r="T12" s="18"/>
+      <c r="U12" s="18"/>
+      <c r="V12" s="18"/>
+      <c r="W12" s="18"/>
+      <c r="X12" s="18"/>
+      <c r="Y12" s="18"/>
+      <c r="Z12" s="18"/>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="18"/>
+      <c r="AC12" s="18"/>
+      <c r="AD12" s="18"/>
+      <c r="AE12" s="18"/>
+      <c r="AF12" s="18"/>
+      <c r="AG12" s="18"/>
+      <c r="AH12" s="18"/>
+      <c r="AI12" s="18"/>
+      <c r="AJ12" s="18"/>
+      <c r="AK12" s="18"/>
+      <c r="AL12" s="19"/>
       <c r="AM12" s="1"/>
       <c r="AN12" s="1"/>
       <c r="AO12" s="1"/>
@@ -1666,50 +1666,50 @@
       <c r="AR12" s="1"/>
     </row>
     <row r="13" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="A13" s="20">
         <v>8</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="27"/>
-      <c r="L13" s="27"/>
-      <c r="M13" s="27"/>
-      <c r="N13" s="27"/>
-      <c r="O13" s="27"/>
-      <c r="P13" s="27"/>
-      <c r="Q13" s="27"/>
-      <c r="R13" s="27"/>
-      <c r="S13" s="27"/>
-      <c r="T13" s="27"/>
-      <c r="U13" s="27"/>
-      <c r="V13" s="27"/>
-      <c r="W13" s="27"/>
-      <c r="X13" s="27"/>
-      <c r="Y13" s="27"/>
-      <c r="Z13" s="27"/>
-      <c r="AA13" s="27"/>
-      <c r="AB13" s="27"/>
-      <c r="AC13" s="27"/>
-      <c r="AD13" s="27"/>
-      <c r="AE13" s="27"/>
-      <c r="AF13" s="27"/>
-      <c r="AG13" s="27"/>
-      <c r="AH13" s="27"/>
-      <c r="AI13" s="27"/>
-      <c r="AJ13" s="27"/>
-      <c r="AK13" s="27"/>
-      <c r="AL13" s="28"/>
+      <c r="D13" s="18"/>
+      <c r="E13" s="18"/>
+      <c r="F13" s="18"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="16"/>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16"/>
+      <c r="K13" s="18"/>
+      <c r="L13" s="18"/>
+      <c r="M13" s="18"/>
+      <c r="N13" s="18"/>
+      <c r="O13" s="18"/>
+      <c r="P13" s="18"/>
+      <c r="Q13" s="18"/>
+      <c r="R13" s="18"/>
+      <c r="S13" s="18"/>
+      <c r="T13" s="18"/>
+      <c r="U13" s="18"/>
+      <c r="V13" s="18"/>
+      <c r="W13" s="18"/>
+      <c r="X13" s="18"/>
+      <c r="Y13" s="18"/>
+      <c r="Z13" s="18"/>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="18"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="18"/>
+      <c r="AE13" s="18"/>
+      <c r="AF13" s="18"/>
+      <c r="AG13" s="18"/>
+      <c r="AH13" s="18"/>
+      <c r="AI13" s="18"/>
+      <c r="AJ13" s="18"/>
+      <c r="AK13" s="18"/>
+      <c r="AL13" s="19"/>
       <c r="AM13" s="1"/>
       <c r="AN13" s="1"/>
       <c r="AO13" s="1"/>
@@ -1718,50 +1718,50 @@
       <c r="AR13" s="1"/>
     </row>
     <row r="14" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A14" s="22">
+      <c r="A14" s="13">
         <v>9</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="31"/>
-      <c r="I14" s="31"/>
-      <c r="J14" s="31"/>
-      <c r="K14" s="31"/>
-      <c r="L14" s="26"/>
-      <c r="M14" s="26"/>
-      <c r="N14" s="26"/>
-      <c r="O14" s="26"/>
-      <c r="P14" s="26"/>
-      <c r="Q14" s="26"/>
-      <c r="R14" s="26"/>
-      <c r="S14" s="26"/>
-      <c r="T14" s="26"/>
-      <c r="U14" s="26"/>
-      <c r="V14" s="26"/>
-      <c r="W14" s="26"/>
-      <c r="X14" s="26"/>
-      <c r="Y14" s="26"/>
-      <c r="Z14" s="27"/>
-      <c r="AA14" s="27"/>
-      <c r="AB14" s="27"/>
-      <c r="AC14" s="27"/>
-      <c r="AD14" s="27"/>
-      <c r="AE14" s="27"/>
-      <c r="AF14" s="27"/>
-      <c r="AG14" s="27"/>
-      <c r="AH14" s="27"/>
-      <c r="AI14" s="27"/>
-      <c r="AJ14" s="27"/>
-      <c r="AK14" s="27"/>
-      <c r="AL14" s="28"/>
+      <c r="D14" s="18"/>
+      <c r="E14" s="18"/>
+      <c r="F14" s="18"/>
+      <c r="G14" s="18"/>
+      <c r="H14" s="22"/>
+      <c r="I14" s="22"/>
+      <c r="J14" s="22"/>
+      <c r="K14" s="22"/>
+      <c r="L14" s="17"/>
+      <c r="M14" s="17"/>
+      <c r="N14" s="17"/>
+      <c r="O14" s="17"/>
+      <c r="P14" s="17"/>
+      <c r="Q14" s="17"/>
+      <c r="R14" s="17"/>
+      <c r="S14" s="17"/>
+      <c r="T14" s="17"/>
+      <c r="U14" s="17"/>
+      <c r="V14" s="17"/>
+      <c r="W14" s="17"/>
+      <c r="X14" s="17"/>
+      <c r="Y14" s="17"/>
+      <c r="Z14" s="18"/>
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="18"/>
+      <c r="AC14" s="18"/>
+      <c r="AD14" s="18"/>
+      <c r="AE14" s="18"/>
+      <c r="AF14" s="18"/>
+      <c r="AG14" s="18"/>
+      <c r="AH14" s="18"/>
+      <c r="AI14" s="18"/>
+      <c r="AJ14" s="18"/>
+      <c r="AK14" s="18"/>
+      <c r="AL14" s="19"/>
       <c r="AM14" s="1"/>
       <c r="AN14" s="1"/>
       <c r="AO14" s="1"/>
@@ -1770,50 +1770,50 @@
       <c r="AR14" s="1"/>
     </row>
     <row r="15" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A15" s="22">
+      <c r="A15" s="13">
         <v>10</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27"/>
-      <c r="K15" s="25"/>
-      <c r="L15" s="25"/>
-      <c r="M15" s="25"/>
-      <c r="N15" s="25"/>
-      <c r="O15" s="25"/>
-      <c r="P15" s="25"/>
-      <c r="Q15" s="33"/>
-      <c r="R15" s="33"/>
-      <c r="S15" s="26"/>
-      <c r="T15" s="26"/>
-      <c r="U15" s="27"/>
-      <c r="V15" s="27"/>
-      <c r="W15" s="27"/>
-      <c r="X15" s="27"/>
-      <c r="Y15" s="27"/>
-      <c r="Z15" s="27"/>
-      <c r="AA15" s="27"/>
-      <c r="AB15" s="27"/>
-      <c r="AC15" s="27"/>
-      <c r="AD15" s="27"/>
-      <c r="AE15" s="27"/>
-      <c r="AF15" s="27"/>
-      <c r="AG15" s="27"/>
-      <c r="AH15" s="27"/>
-      <c r="AI15" s="27"/>
-      <c r="AJ15" s="27"/>
-      <c r="AK15" s="27"/>
-      <c r="AL15" s="28"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="16"/>
+      <c r="N15" s="16"/>
+      <c r="O15" s="16"/>
+      <c r="P15" s="16"/>
+      <c r="Q15" s="24"/>
+      <c r="R15" s="24"/>
+      <c r="S15" s="17"/>
+      <c r="T15" s="17"/>
+      <c r="U15" s="18"/>
+      <c r="V15" s="18"/>
+      <c r="W15" s="18"/>
+      <c r="X15" s="18"/>
+      <c r="Y15" s="18"/>
+      <c r="Z15" s="18"/>
+      <c r="AA15" s="18"/>
+      <c r="AB15" s="18"/>
+      <c r="AC15" s="18"/>
+      <c r="AD15" s="18"/>
+      <c r="AE15" s="18"/>
+      <c r="AF15" s="18"/>
+      <c r="AG15" s="18"/>
+      <c r="AH15" s="18"/>
+      <c r="AI15" s="18"/>
+      <c r="AJ15" s="18"/>
+      <c r="AK15" s="18"/>
+      <c r="AL15" s="19"/>
       <c r="AM15" s="1"/>
       <c r="AN15" s="1"/>
       <c r="AO15" s="1"/>
@@ -1822,50 +1822,50 @@
       <c r="AR15" s="1"/>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A16" s="29">
+      <c r="A16" s="20">
         <v>11</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="25"/>
-      <c r="N16" s="25"/>
-      <c r="O16" s="25"/>
-      <c r="P16" s="25"/>
-      <c r="Q16" s="33"/>
-      <c r="R16" s="33"/>
-      <c r="S16" s="26"/>
-      <c r="T16" s="26"/>
-      <c r="U16" s="27"/>
-      <c r="V16" s="27"/>
-      <c r="W16" s="27"/>
-      <c r="X16" s="27"/>
-      <c r="Y16" s="27"/>
-      <c r="Z16" s="27"/>
-      <c r="AA16" s="27"/>
-      <c r="AB16" s="27"/>
-      <c r="AC16" s="27"/>
-      <c r="AD16" s="27"/>
-      <c r="AE16" s="27"/>
-      <c r="AF16" s="27"/>
-      <c r="AG16" s="27"/>
-      <c r="AH16" s="27"/>
-      <c r="AI16" s="27"/>
-      <c r="AJ16" s="27"/>
-      <c r="AK16" s="27"/>
-      <c r="AL16" s="28"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16"/>
+      <c r="M16" s="16"/>
+      <c r="N16" s="16"/>
+      <c r="O16" s="16"/>
+      <c r="P16" s="16"/>
+      <c r="Q16" s="24"/>
+      <c r="R16" s="24"/>
+      <c r="S16" s="17"/>
+      <c r="T16" s="17"/>
+      <c r="U16" s="18"/>
+      <c r="V16" s="18"/>
+      <c r="W16" s="18"/>
+      <c r="X16" s="18"/>
+      <c r="Y16" s="18"/>
+      <c r="Z16" s="18"/>
+      <c r="AA16" s="18"/>
+      <c r="AB16" s="18"/>
+      <c r="AC16" s="18"/>
+      <c r="AD16" s="18"/>
+      <c r="AE16" s="18"/>
+      <c r="AF16" s="18"/>
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="18"/>
+      <c r="AI16" s="18"/>
+      <c r="AJ16" s="18"/>
+      <c r="AK16" s="18"/>
+      <c r="AL16" s="19"/>
       <c r="AM16" s="1"/>
       <c r="AN16" s="1"/>
       <c r="AO16" s="1"/>
@@ -1874,50 +1874,50 @@
       <c r="AR16" s="1"/>
     </row>
     <row r="17" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A17" s="22">
+      <c r="A17" s="13">
         <v>12</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="24" t="s">
+      <c r="C17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="26"/>
-      <c r="L17" s="31"/>
-      <c r="M17" s="31"/>
-      <c r="N17" s="31"/>
-      <c r="O17" s="31"/>
-      <c r="P17" s="31"/>
-      <c r="Q17" s="31"/>
-      <c r="R17" s="31"/>
-      <c r="S17" s="31"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="31"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="31"/>
-      <c r="X17" s="31"/>
-      <c r="Y17" s="31"/>
-      <c r="Z17" s="27"/>
-      <c r="AA17" s="27"/>
-      <c r="AB17" s="27"/>
-      <c r="AC17" s="27"/>
-      <c r="AD17" s="27"/>
-      <c r="AE17" s="27"/>
-      <c r="AF17" s="27"/>
-      <c r="AG17" s="27"/>
-      <c r="AH17" s="27"/>
-      <c r="AI17" s="27"/>
-      <c r="AJ17" s="27"/>
-      <c r="AK17" s="27"/>
-      <c r="AL17" s="28"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="18"/>
+      <c r="F17" s="18"/>
+      <c r="G17" s="18"/>
+      <c r="H17" s="18"/>
+      <c r="I17" s="18"/>
+      <c r="J17" s="18"/>
+      <c r="K17" s="17"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
+      <c r="V17" s="22"/>
+      <c r="W17" s="22"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+      <c r="Z17" s="18"/>
+      <c r="AA17" s="18"/>
+      <c r="AB17" s="18"/>
+      <c r="AC17" s="18"/>
+      <c r="AD17" s="18"/>
+      <c r="AE17" s="18"/>
+      <c r="AF17" s="18"/>
+      <c r="AG17" s="18"/>
+      <c r="AH17" s="18"/>
+      <c r="AI17" s="18"/>
+      <c r="AJ17" s="18"/>
+      <c r="AK17" s="18"/>
+      <c r="AL17" s="19"/>
       <c r="AM17" s="1"/>
       <c r="AN17" s="1"/>
       <c r="AO17" s="1"/>
@@ -1926,50 +1926,50 @@
       <c r="AR17" s="1"/>
     </row>
     <row r="18" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A18" s="22">
+      <c r="A18" s="13">
         <v>13</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
-      <c r="J18" s="27"/>
-      <c r="K18" s="26"/>
-      <c r="L18" s="26"/>
-      <c r="M18" s="26"/>
-      <c r="N18" s="26"/>
-      <c r="O18" s="26"/>
-      <c r="P18" s="26"/>
-      <c r="Q18" s="31"/>
-      <c r="R18" s="31"/>
-      <c r="S18" s="31"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="31"/>
-      <c r="X18" s="31"/>
-      <c r="Y18" s="31"/>
-      <c r="Z18" s="27"/>
-      <c r="AA18" s="27"/>
-      <c r="AB18" s="27"/>
-      <c r="AC18" s="27"/>
-      <c r="AD18" s="27"/>
-      <c r="AE18" s="27"/>
-      <c r="AF18" s="27"/>
-      <c r="AG18" s="27"/>
-      <c r="AH18" s="27"/>
-      <c r="AI18" s="27"/>
-      <c r="AJ18" s="27"/>
-      <c r="AK18" s="27"/>
-      <c r="AL18" s="28"/>
+      <c r="D18" s="18"/>
+      <c r="E18" s="18"/>
+      <c r="F18" s="18"/>
+      <c r="G18" s="18"/>
+      <c r="H18" s="18"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="18"/>
+      <c r="K18" s="17"/>
+      <c r="L18" s="17"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="17"/>
+      <c r="O18" s="17"/>
+      <c r="P18" s="17"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="22"/>
+      <c r="S18" s="22"/>
+      <c r="T18" s="22"/>
+      <c r="U18" s="22"/>
+      <c r="V18" s="22"/>
+      <c r="W18" s="22"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
+      <c r="Z18" s="18"/>
+      <c r="AA18" s="18"/>
+      <c r="AB18" s="18"/>
+      <c r="AC18" s="18"/>
+      <c r="AD18" s="18"/>
+      <c r="AE18" s="18"/>
+      <c r="AF18" s="18"/>
+      <c r="AG18" s="18"/>
+      <c r="AH18" s="18"/>
+      <c r="AI18" s="18"/>
+      <c r="AJ18" s="18"/>
+      <c r="AK18" s="18"/>
+      <c r="AL18" s="19"/>
       <c r="AM18" s="1"/>
       <c r="AN18" s="1"/>
       <c r="AO18" s="1"/>
@@ -1978,50 +1978,50 @@
       <c r="AR18" s="1"/>
     </row>
     <row r="19" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A19" s="29">
+      <c r="A19" s="20">
         <v>14</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="24" t="s">
+      <c r="C19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
-      <c r="J19" s="27"/>
-      <c r="K19" s="26"/>
-      <c r="L19" s="26"/>
-      <c r="M19" s="26"/>
-      <c r="N19" s="26"/>
-      <c r="O19" s="26"/>
-      <c r="P19" s="26"/>
-      <c r="Q19" s="25"/>
-      <c r="R19" s="25"/>
-      <c r="S19" s="26"/>
-      <c r="T19" s="26"/>
-      <c r="U19" s="26"/>
-      <c r="V19" s="26"/>
-      <c r="W19" s="26"/>
-      <c r="X19" s="26"/>
-      <c r="Y19" s="26"/>
-      <c r="Z19" s="26"/>
-      <c r="AA19" s="27"/>
-      <c r="AB19" s="27"/>
-      <c r="AC19" s="27"/>
-      <c r="AD19" s="27"/>
-      <c r="AE19" s="27"/>
-      <c r="AF19" s="27"/>
-      <c r="AG19" s="27"/>
-      <c r="AH19" s="27"/>
-      <c r="AI19" s="27"/>
-      <c r="AJ19" s="27"/>
-      <c r="AK19" s="27"/>
-      <c r="AL19" s="28"/>
+      <c r="D19" s="18"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="18"/>
+      <c r="G19" s="18"/>
+      <c r="H19" s="18"/>
+      <c r="I19" s="18"/>
+      <c r="J19" s="18"/>
+      <c r="K19" s="17"/>
+      <c r="L19" s="17"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="17"/>
+      <c r="O19" s="17"/>
+      <c r="P19" s="17"/>
+      <c r="Q19" s="16"/>
+      <c r="R19" s="16"/>
+      <c r="S19" s="17"/>
+      <c r="T19" s="17"/>
+      <c r="U19" s="17"/>
+      <c r="V19" s="17"/>
+      <c r="W19" s="17"/>
+      <c r="X19" s="17"/>
+      <c r="Y19" s="17"/>
+      <c r="Z19" s="17"/>
+      <c r="AA19" s="18"/>
+      <c r="AB19" s="18"/>
+      <c r="AC19" s="18"/>
+      <c r="AD19" s="18"/>
+      <c r="AE19" s="18"/>
+      <c r="AF19" s="18"/>
+      <c r="AG19" s="18"/>
+      <c r="AH19" s="18"/>
+      <c r="AI19" s="18"/>
+      <c r="AJ19" s="18"/>
+      <c r="AK19" s="18"/>
+      <c r="AL19" s="19"/>
       <c r="AM19" s="1"/>
       <c r="AN19" s="1"/>
       <c r="AO19" s="1"/>
@@ -2030,50 +2030,50 @@
       <c r="AR19" s="1"/>
     </row>
     <row r="20" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A20" s="22">
+      <c r="A20" s="13">
         <v>15</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
-      <c r="L20" s="27"/>
-      <c r="M20" s="27"/>
-      <c r="N20" s="27"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="27"/>
-      <c r="Q20" s="27"/>
-      <c r="R20" s="27"/>
-      <c r="S20" s="25"/>
-      <c r="T20" s="25"/>
-      <c r="U20" s="25"/>
-      <c r="V20" s="25"/>
-      <c r="W20" s="25"/>
-      <c r="X20" s="26"/>
-      <c r="Y20" s="26"/>
-      <c r="Z20" s="27"/>
-      <c r="AA20" s="27"/>
-      <c r="AB20" s="27"/>
-      <c r="AC20" s="27"/>
-      <c r="AD20" s="26"/>
-      <c r="AE20" s="26"/>
-      <c r="AF20" s="26"/>
-      <c r="AG20" s="26"/>
-      <c r="AH20" s="26"/>
-      <c r="AI20" s="27"/>
-      <c r="AJ20" s="27"/>
-      <c r="AK20" s="27"/>
-      <c r="AL20" s="28"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
+      <c r="H20" s="18"/>
+      <c r="I20" s="18"/>
+      <c r="J20" s="18"/>
+      <c r="K20" s="18"/>
+      <c r="L20" s="18"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="18"/>
+      <c r="O20" s="18"/>
+      <c r="P20" s="18"/>
+      <c r="Q20" s="18"/>
+      <c r="R20" s="18"/>
+      <c r="S20" s="16"/>
+      <c r="T20" s="16"/>
+      <c r="U20" s="16"/>
+      <c r="V20" s="16"/>
+      <c r="W20" s="16"/>
+      <c r="X20" s="16"/>
+      <c r="Y20" s="17"/>
+      <c r="Z20" s="18"/>
+      <c r="AA20" s="18"/>
+      <c r="AB20" s="18"/>
+      <c r="AC20" s="18"/>
+      <c r="AD20" s="17"/>
+      <c r="AE20" s="17"/>
+      <c r="AF20" s="17"/>
+      <c r="AG20" s="17"/>
+      <c r="AH20" s="17"/>
+      <c r="AI20" s="18"/>
+      <c r="AJ20" s="18"/>
+      <c r="AK20" s="18"/>
+      <c r="AL20" s="19"/>
       <c r="AM20" s="1"/>
       <c r="AN20" s="1"/>
       <c r="AO20" s="1"/>
@@ -2082,50 +2082,50 @@
       <c r="AR20" s="1"/>
     </row>
     <row r="21" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A21" s="22">
+      <c r="A21" s="13">
         <v>16</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="C21" s="24" t="s">
+      <c r="C21" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
-      <c r="L21" s="27"/>
-      <c r="M21" s="27"/>
-      <c r="N21" s="27"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="27"/>
-      <c r="Q21" s="27"/>
-      <c r="R21" s="27"/>
-      <c r="S21" s="26"/>
-      <c r="T21" s="26"/>
-      <c r="U21" s="26"/>
-      <c r="V21" s="26"/>
-      <c r="W21" s="26"/>
-      <c r="X21" s="25"/>
-      <c r="Y21" s="25"/>
-      <c r="Z21" s="27"/>
-      <c r="AA21" s="27"/>
-      <c r="AB21" s="27"/>
-      <c r="AC21" s="27"/>
-      <c r="AD21" s="26"/>
-      <c r="AE21" s="26"/>
-      <c r="AF21" s="26"/>
-      <c r="AG21" s="26"/>
-      <c r="AH21" s="26"/>
-      <c r="AI21" s="27"/>
-      <c r="AJ21" s="27"/>
-      <c r="AK21" s="27"/>
-      <c r="AL21" s="28"/>
+      <c r="D21" s="18"/>
+      <c r="E21" s="18"/>
+      <c r="F21" s="18"/>
+      <c r="G21" s="18"/>
+      <c r="H21" s="18"/>
+      <c r="I21" s="18"/>
+      <c r="J21" s="18"/>
+      <c r="K21" s="18"/>
+      <c r="L21" s="18"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="18"/>
+      <c r="O21" s="18"/>
+      <c r="P21" s="18"/>
+      <c r="Q21" s="18"/>
+      <c r="R21" s="18"/>
+      <c r="S21" s="17"/>
+      <c r="T21" s="17"/>
+      <c r="U21" s="17"/>
+      <c r="V21" s="17"/>
+      <c r="W21" s="17"/>
+      <c r="X21" s="17"/>
+      <c r="Y21" s="16"/>
+      <c r="Z21" s="18"/>
+      <c r="AA21" s="18"/>
+      <c r="AB21" s="18"/>
+      <c r="AC21" s="18"/>
+      <c r="AD21" s="17"/>
+      <c r="AE21" s="17"/>
+      <c r="AF21" s="17"/>
+      <c r="AG21" s="17"/>
+      <c r="AH21" s="17"/>
+      <c r="AI21" s="18"/>
+      <c r="AJ21" s="18"/>
+      <c r="AK21" s="18"/>
+      <c r="AL21" s="19"/>
       <c r="AM21" s="1"/>
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
@@ -2134,50 +2134,50 @@
       <c r="AR21" s="1"/>
     </row>
     <row r="22" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A22" s="29">
+      <c r="A22" s="20">
         <v>17</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="26"/>
-      <c r="E22" s="26"/>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="26"/>
-      <c r="I22" s="26"/>
-      <c r="J22" s="26"/>
-      <c r="K22" s="27"/>
-      <c r="L22" s="27"/>
-      <c r="M22" s="27"/>
-      <c r="N22" s="27"/>
-      <c r="O22" s="27"/>
-      <c r="P22" s="27"/>
-      <c r="Q22" s="27"/>
-      <c r="R22" s="27"/>
-      <c r="S22" s="27"/>
-      <c r="T22" s="27"/>
-      <c r="U22" s="27"/>
-      <c r="V22" s="27"/>
-      <c r="W22" s="27"/>
-      <c r="X22" s="27"/>
-      <c r="Y22" s="27"/>
-      <c r="Z22" s="31"/>
-      <c r="AA22" s="31"/>
-      <c r="AB22" s="26"/>
-      <c r="AC22" s="27"/>
-      <c r="AD22" s="27"/>
-      <c r="AE22" s="27"/>
-      <c r="AF22" s="27"/>
-      <c r="AG22" s="27"/>
-      <c r="AH22" s="27"/>
-      <c r="AI22" s="27"/>
-      <c r="AJ22" s="27"/>
-      <c r="AK22" s="27"/>
-      <c r="AL22" s="28"/>
+      <c r="D22" s="17"/>
+      <c r="E22" s="17"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+      <c r="K22" s="18"/>
+      <c r="L22" s="18"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="18"/>
+      <c r="P22" s="18"/>
+      <c r="Q22" s="18"/>
+      <c r="R22" s="18"/>
+      <c r="S22" s="18"/>
+      <c r="T22" s="18"/>
+      <c r="U22" s="18"/>
+      <c r="V22" s="18"/>
+      <c r="W22" s="18"/>
+      <c r="X22" s="18"/>
+      <c r="Y22" s="18"/>
+      <c r="Z22" s="22"/>
+      <c r="AA22" s="22"/>
+      <c r="AB22" s="17"/>
+      <c r="AC22" s="18"/>
+      <c r="AD22" s="18"/>
+      <c r="AE22" s="18"/>
+      <c r="AF22" s="18"/>
+      <c r="AG22" s="18"/>
+      <c r="AH22" s="18"/>
+      <c r="AI22" s="18"/>
+      <c r="AJ22" s="18"/>
+      <c r="AK22" s="18"/>
+      <c r="AL22" s="19"/>
       <c r="AN22" s="1"/>
       <c r="AO22" s="1"/>
       <c r="AP22" s="1"/>
@@ -2185,50 +2185,50 @@
       <c r="AR22" s="1"/>
     </row>
     <row r="23" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A23" s="22">
+      <c r="A23" s="13">
         <v>18</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C23" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="26"/>
-      <c r="E23" s="26"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="26"/>
-      <c r="I23" s="26"/>
-      <c r="J23" s="26"/>
-      <c r="K23" s="27"/>
-      <c r="L23" s="27"/>
-      <c r="M23" s="27"/>
-      <c r="N23" s="27"/>
-      <c r="O23" s="27"/>
-      <c r="P23" s="27"/>
-      <c r="Q23" s="27"/>
-      <c r="R23" s="27"/>
-      <c r="S23" s="27"/>
-      <c r="T23" s="27"/>
-      <c r="U23" s="27"/>
-      <c r="V23" s="27"/>
-      <c r="W23" s="27"/>
-      <c r="X23" s="27"/>
-      <c r="Y23" s="27"/>
-      <c r="Z23" s="31"/>
-      <c r="AA23" s="31"/>
-      <c r="AB23" s="26"/>
-      <c r="AC23" s="27"/>
-      <c r="AD23" s="27"/>
-      <c r="AE23" s="27"/>
-      <c r="AF23" s="27"/>
-      <c r="AG23" s="27"/>
-      <c r="AH23" s="27"/>
-      <c r="AI23" s="27"/>
-      <c r="AJ23" s="27"/>
-      <c r="AK23" s="27"/>
-      <c r="AL23" s="28"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="18"/>
+      <c r="G23" s="18"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="18"/>
+      <c r="L23" s="18"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="18"/>
+      <c r="O23" s="18"/>
+      <c r="P23" s="18"/>
+      <c r="Q23" s="18"/>
+      <c r="R23" s="18"/>
+      <c r="S23" s="18"/>
+      <c r="T23" s="18"/>
+      <c r="U23" s="18"/>
+      <c r="V23" s="18"/>
+      <c r="W23" s="18"/>
+      <c r="X23" s="18"/>
+      <c r="Y23" s="18"/>
+      <c r="Z23" s="22"/>
+      <c r="AA23" s="22"/>
+      <c r="AB23" s="17"/>
+      <c r="AC23" s="18"/>
+      <c r="AD23" s="18"/>
+      <c r="AE23" s="18"/>
+      <c r="AF23" s="18"/>
+      <c r="AG23" s="18"/>
+      <c r="AH23" s="18"/>
+      <c r="AI23" s="18"/>
+      <c r="AJ23" s="18"/>
+      <c r="AK23" s="18"/>
+      <c r="AL23" s="19"/>
       <c r="AN23" s="1"/>
       <c r="AO23" s="1"/>
       <c r="AP23" s="1"/>
@@ -2236,50 +2236,50 @@
       <c r="AR23" s="1"/>
     </row>
     <row r="24" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A24" s="22">
+      <c r="A24" s="13">
         <v>19</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="D24" s="27"/>
-      <c r="E24" s="27"/>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="27"/>
-      <c r="L24" s="27"/>
-      <c r="M24" s="27"/>
-      <c r="N24" s="27"/>
-      <c r="O24" s="27"/>
-      <c r="P24" s="27"/>
-      <c r="Q24" s="27"/>
-      <c r="R24" s="27"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="26"/>
-      <c r="Y24" s="26"/>
-      <c r="Z24" s="25"/>
-      <c r="AA24" s="25"/>
-      <c r="AB24" s="25"/>
-      <c r="AC24" s="25"/>
-      <c r="AD24" s="25"/>
-      <c r="AE24" s="27"/>
-      <c r="AF24" s="27"/>
-      <c r="AG24" s="27"/>
-      <c r="AH24" s="27"/>
-      <c r="AI24" s="27"/>
-      <c r="AJ24" s="27"/>
-      <c r="AK24" s="27"/>
-      <c r="AL24" s="28"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="17"/>
+      <c r="I24" s="17"/>
+      <c r="J24" s="17"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="18"/>
+      <c r="O24" s="18"/>
+      <c r="P24" s="18"/>
+      <c r="Q24" s="18"/>
+      <c r="R24" s="18"/>
+      <c r="S24" s="17"/>
+      <c r="T24" s="17"/>
+      <c r="U24" s="17"/>
+      <c r="V24" s="17"/>
+      <c r="W24" s="17"/>
+      <c r="X24" s="17"/>
+      <c r="Y24" s="17"/>
+      <c r="Z24" s="16"/>
+      <c r="AA24" s="16"/>
+      <c r="AB24" s="16"/>
+      <c r="AC24" s="16"/>
+      <c r="AD24" s="16"/>
+      <c r="AE24" s="18"/>
+      <c r="AF24" s="18"/>
+      <c r="AG24" s="18"/>
+      <c r="AH24" s="18"/>
+      <c r="AI24" s="18"/>
+      <c r="AJ24" s="18"/>
+      <c r="AK24" s="18"/>
+      <c r="AL24" s="19"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
       <c r="AO24" s="1"/>
@@ -2288,50 +2288,50 @@
       <c r="AR24" s="1"/>
     </row>
     <row r="25" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A25" s="29">
+      <c r="A25" s="20">
         <v>20</v>
       </c>
-      <c r="B25" s="34" t="s">
+      <c r="B25" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="D25" s="27"/>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="26"/>
-      <c r="I25" s="26"/>
-      <c r="J25" s="26"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="27"/>
-      <c r="M25" s="27"/>
-      <c r="N25" s="27"/>
-      <c r="O25" s="27"/>
-      <c r="P25" s="27"/>
-      <c r="Q25" s="27"/>
-      <c r="R25" s="27"/>
-      <c r="S25" s="26"/>
-      <c r="T25" s="26"/>
-      <c r="U25" s="26"/>
-      <c r="V25" s="26"/>
-      <c r="W25" s="26"/>
-      <c r="X25" s="26"/>
-      <c r="Y25" s="26"/>
-      <c r="Z25" s="26"/>
-      <c r="AA25" s="26"/>
-      <c r="AB25" s="31"/>
-      <c r="AC25" s="26"/>
-      <c r="AD25" s="26"/>
-      <c r="AE25" s="27"/>
-      <c r="AF25" s="27"/>
-      <c r="AG25" s="27"/>
-      <c r="AH25" s="27"/>
-      <c r="AI25" s="27"/>
-      <c r="AJ25" s="27"/>
-      <c r="AK25" s="27"/>
-      <c r="AL25" s="28"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="18"/>
+      <c r="O25" s="18"/>
+      <c r="P25" s="18"/>
+      <c r="Q25" s="18"/>
+      <c r="R25" s="18"/>
+      <c r="S25" s="17"/>
+      <c r="T25" s="17"/>
+      <c r="U25" s="17"/>
+      <c r="V25" s="17"/>
+      <c r="W25" s="17"/>
+      <c r="X25" s="17"/>
+      <c r="Y25" s="17"/>
+      <c r="Z25" s="17"/>
+      <c r="AA25" s="17"/>
+      <c r="AB25" s="22"/>
+      <c r="AC25" s="17"/>
+      <c r="AD25" s="17"/>
+      <c r="AE25" s="18"/>
+      <c r="AF25" s="18"/>
+      <c r="AG25" s="18"/>
+      <c r="AH25" s="18"/>
+      <c r="AI25" s="18"/>
+      <c r="AJ25" s="18"/>
+      <c r="AK25" s="18"/>
+      <c r="AL25" s="19"/>
       <c r="AM25" s="1"/>
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
@@ -2340,50 +2340,50 @@
       <c r="AR25" s="1"/>
     </row>
     <row r="26" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A26" s="22">
+      <c r="A26" s="13">
         <v>21</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="27"/>
-      <c r="M26" s="27"/>
-      <c r="N26" s="27"/>
-      <c r="O26" s="27"/>
-      <c r="P26" s="27"/>
-      <c r="Q26" s="27"/>
-      <c r="R26" s="27"/>
-      <c r="S26" s="27"/>
-      <c r="T26" s="27"/>
-      <c r="U26" s="27"/>
-      <c r="V26" s="27"/>
-      <c r="W26" s="27"/>
-      <c r="X26" s="27"/>
-      <c r="Y26" s="27"/>
-      <c r="Z26" s="26"/>
-      <c r="AA26" s="26"/>
-      <c r="AB26" s="26"/>
-      <c r="AC26" s="31"/>
-      <c r="AD26" s="27"/>
-      <c r="AE26" s="27"/>
-      <c r="AF26" s="27"/>
-      <c r="AG26" s="27"/>
-      <c r="AH26" s="27"/>
-      <c r="AI26" s="27"/>
-      <c r="AJ26" s="27"/>
-      <c r="AK26" s="27"/>
-      <c r="AL26" s="28"/>
+      <c r="D26" s="18"/>
+      <c r="E26" s="18"/>
+      <c r="F26" s="18"/>
+      <c r="G26" s="18"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="18"/>
+      <c r="P26" s="18"/>
+      <c r="Q26" s="18"/>
+      <c r="R26" s="18"/>
+      <c r="S26" s="18"/>
+      <c r="T26" s="18"/>
+      <c r="U26" s="18"/>
+      <c r="V26" s="18"/>
+      <c r="W26" s="18"/>
+      <c r="X26" s="18"/>
+      <c r="Y26" s="18"/>
+      <c r="Z26" s="17"/>
+      <c r="AA26" s="17"/>
+      <c r="AB26" s="17"/>
+      <c r="AC26" s="22"/>
+      <c r="AD26" s="18"/>
+      <c r="AE26" s="18"/>
+      <c r="AF26" s="18"/>
+      <c r="AG26" s="18"/>
+      <c r="AH26" s="18"/>
+      <c r="AI26" s="18"/>
+      <c r="AJ26" s="18"/>
+      <c r="AK26" s="18"/>
+      <c r="AL26" s="19"/>
       <c r="AM26" s="1"/>
       <c r="AN26" s="1"/>
       <c r="AO26" s="1"/>
@@ -2392,50 +2392,50 @@
       <c r="AR26" s="1"/>
     </row>
     <row r="27" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A27" s="22">
+      <c r="A27" s="13">
         <v>22</v>
       </c>
-      <c r="B27" s="34" t="s">
+      <c r="B27" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C27" s="24" t="s">
+      <c r="C27" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D27" s="27"/>
-      <c r="E27" s="27"/>
-      <c r="F27" s="27"/>
-      <c r="G27" s="27"/>
-      <c r="H27" s="27"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="27"/>
-      <c r="M27" s="27"/>
-      <c r="N27" s="27"/>
-      <c r="O27" s="27"/>
-      <c r="P27" s="27"/>
-      <c r="Q27" s="27"/>
-      <c r="R27" s="27"/>
-      <c r="S27" s="27"/>
-      <c r="T27" s="27"/>
-      <c r="U27" s="27"/>
-      <c r="V27" s="27"/>
-      <c r="W27" s="27"/>
-      <c r="X27" s="27"/>
-      <c r="Y27" s="27"/>
-      <c r="Z27" s="26"/>
-      <c r="AA27" s="26"/>
-      <c r="AB27" s="26"/>
-      <c r="AC27" s="26"/>
-      <c r="AD27" s="31"/>
-      <c r="AE27" s="27"/>
-      <c r="AF27" s="27"/>
-      <c r="AG27" s="27"/>
-      <c r="AH27" s="27"/>
-      <c r="AI27" s="27"/>
-      <c r="AJ27" s="27"/>
-      <c r="AK27" s="27"/>
-      <c r="AL27" s="28"/>
+      <c r="D27" s="18"/>
+      <c r="E27" s="18"/>
+      <c r="F27" s="18"/>
+      <c r="G27" s="18"/>
+      <c r="H27" s="18"/>
+      <c r="I27" s="18"/>
+      <c r="J27" s="18"/>
+      <c r="K27" s="18"/>
+      <c r="L27" s="18"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="18"/>
+      <c r="O27" s="18"/>
+      <c r="P27" s="18"/>
+      <c r="Q27" s="18"/>
+      <c r="R27" s="18"/>
+      <c r="S27" s="18"/>
+      <c r="T27" s="18"/>
+      <c r="U27" s="18"/>
+      <c r="V27" s="18"/>
+      <c r="W27" s="18"/>
+      <c r="X27" s="18"/>
+      <c r="Y27" s="18"/>
+      <c r="Z27" s="17"/>
+      <c r="AA27" s="17"/>
+      <c r="AB27" s="17"/>
+      <c r="AC27" s="17"/>
+      <c r="AD27" s="22"/>
+      <c r="AE27" s="18"/>
+      <c r="AF27" s="18"/>
+      <c r="AG27" s="18"/>
+      <c r="AH27" s="18"/>
+      <c r="AI27" s="18"/>
+      <c r="AJ27" s="18"/>
+      <c r="AK27" s="18"/>
+      <c r="AL27" s="19"/>
       <c r="AM27" s="1"/>
       <c r="AN27" s="1"/>
       <c r="AO27" s="1"/>
@@ -2444,50 +2444,50 @@
       <c r="AR27" s="1"/>
     </row>
     <row r="28" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A28" s="29">
+      <c r="A28" s="20">
         <v>23</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C28" s="24" t="s">
+      <c r="C28" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
-      <c r="G28" s="27"/>
-      <c r="H28" s="27"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="27"/>
-      <c r="M28" s="27"/>
-      <c r="N28" s="27"/>
-      <c r="O28" s="27"/>
-      <c r="P28" s="27"/>
-      <c r="Q28" s="27"/>
-      <c r="R28" s="27"/>
-      <c r="S28" s="27"/>
-      <c r="T28" s="27"/>
-      <c r="U28" s="27"/>
-      <c r="V28" s="27"/>
-      <c r="W28" s="27"/>
-      <c r="X28" s="27"/>
-      <c r="Y28" s="27"/>
-      <c r="Z28" s="27"/>
-      <c r="AA28" s="27"/>
-      <c r="AB28" s="27"/>
-      <c r="AC28" s="26"/>
-      <c r="AD28" s="26"/>
-      <c r="AE28" s="31"/>
-      <c r="AF28" s="27"/>
-      <c r="AG28" s="27"/>
-      <c r="AH28" s="27"/>
-      <c r="AI28" s="27"/>
-      <c r="AJ28" s="27"/>
-      <c r="AK28" s="27"/>
-      <c r="AL28" s="28"/>
+      <c r="D28" s="18"/>
+      <c r="E28" s="18"/>
+      <c r="F28" s="18"/>
+      <c r="G28" s="18"/>
+      <c r="H28" s="18"/>
+      <c r="I28" s="18"/>
+      <c r="J28" s="18"/>
+      <c r="K28" s="18"/>
+      <c r="L28" s="18"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="18"/>
+      <c r="O28" s="18"/>
+      <c r="P28" s="18"/>
+      <c r="Q28" s="18"/>
+      <c r="R28" s="18"/>
+      <c r="S28" s="18"/>
+      <c r="T28" s="18"/>
+      <c r="U28" s="18"/>
+      <c r="V28" s="18"/>
+      <c r="W28" s="18"/>
+      <c r="X28" s="18"/>
+      <c r="Y28" s="18"/>
+      <c r="Z28" s="18"/>
+      <c r="AA28" s="18"/>
+      <c r="AB28" s="18"/>
+      <c r="AC28" s="17"/>
+      <c r="AD28" s="17"/>
+      <c r="AE28" s="22"/>
+      <c r="AF28" s="18"/>
+      <c r="AG28" s="18"/>
+      <c r="AH28" s="18"/>
+      <c r="AI28" s="18"/>
+      <c r="AJ28" s="18"/>
+      <c r="AK28" s="18"/>
+      <c r="AL28" s="19"/>
       <c r="AM28" s="1"/>
       <c r="AN28" s="1"/>
       <c r="AO28" s="1"/>
@@ -2496,50 +2496,50 @@
       <c r="AR28" s="1"/>
     </row>
     <row r="29" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A29" s="22">
+      <c r="A29" s="13">
         <v>24</v>
       </c>
-      <c r="B29" s="34" t="s">
+      <c r="B29" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C29" s="24" t="s">
+      <c r="C29" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="D29" s="27"/>
-      <c r="E29" s="27"/>
-      <c r="F29" s="27"/>
-      <c r="G29" s="27"/>
-      <c r="H29" s="27"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="27"/>
-      <c r="M29" s="27"/>
-      <c r="N29" s="27"/>
-      <c r="O29" s="27"/>
-      <c r="P29" s="27"/>
-      <c r="Q29" s="27"/>
-      <c r="R29" s="27"/>
-      <c r="S29" s="27"/>
-      <c r="T29" s="27"/>
-      <c r="U29" s="27"/>
-      <c r="V29" s="27"/>
-      <c r="W29" s="27"/>
-      <c r="X29" s="27"/>
-      <c r="Y29" s="27"/>
-      <c r="Z29" s="27"/>
-      <c r="AA29" s="27"/>
-      <c r="AB29" s="27"/>
-      <c r="AC29" s="26"/>
-      <c r="AD29" s="26"/>
-      <c r="AE29" s="26"/>
-      <c r="AF29" s="31"/>
-      <c r="AG29" s="27"/>
-      <c r="AH29" s="27"/>
-      <c r="AI29" s="27"/>
-      <c r="AJ29" s="27"/>
-      <c r="AK29" s="27"/>
-      <c r="AL29" s="28"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="18"/>
+      <c r="G29" s="18"/>
+      <c r="H29" s="18"/>
+      <c r="I29" s="18"/>
+      <c r="J29" s="18"/>
+      <c r="K29" s="18"/>
+      <c r="L29" s="18"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="18"/>
+      <c r="O29" s="18"/>
+      <c r="P29" s="18"/>
+      <c r="Q29" s="18"/>
+      <c r="R29" s="18"/>
+      <c r="S29" s="18"/>
+      <c r="T29" s="18"/>
+      <c r="U29" s="18"/>
+      <c r="V29" s="18"/>
+      <c r="W29" s="18"/>
+      <c r="X29" s="18"/>
+      <c r="Y29" s="18"/>
+      <c r="Z29" s="18"/>
+      <c r="AA29" s="18"/>
+      <c r="AB29" s="18"/>
+      <c r="AC29" s="17"/>
+      <c r="AD29" s="17"/>
+      <c r="AE29" s="17"/>
+      <c r="AF29" s="22"/>
+      <c r="AG29" s="18"/>
+      <c r="AH29" s="18"/>
+      <c r="AI29" s="18"/>
+      <c r="AJ29" s="18"/>
+      <c r="AK29" s="18"/>
+      <c r="AL29" s="19"/>
       <c r="AM29" s="1"/>
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
@@ -2548,50 +2548,50 @@
       <c r="AR29" s="1"/>
     </row>
     <row r="30" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A30" s="22">
+      <c r="A30" s="13">
         <v>25</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="27"/>
-      <c r="H30" s="27"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="27"/>
-      <c r="M30" s="27"/>
-      <c r="N30" s="27"/>
-      <c r="O30" s="27"/>
-      <c r="P30" s="27"/>
-      <c r="Q30" s="27"/>
-      <c r="R30" s="27"/>
-      <c r="S30" s="27"/>
-      <c r="T30" s="27"/>
-      <c r="U30" s="27"/>
-      <c r="V30" s="27"/>
-      <c r="W30" s="27"/>
-      <c r="X30" s="27"/>
-      <c r="Y30" s="27"/>
-      <c r="Z30" s="36"/>
-      <c r="AA30" s="36"/>
-      <c r="AB30" s="36"/>
-      <c r="AC30" s="36"/>
-      <c r="AD30" s="36"/>
-      <c r="AE30" s="36"/>
-      <c r="AF30" s="36"/>
-      <c r="AG30" s="36"/>
-      <c r="AH30" s="36"/>
-      <c r="AI30" s="36"/>
-      <c r="AJ30" s="36"/>
-      <c r="AK30" s="36"/>
-      <c r="AL30" s="37"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+      <c r="F30" s="18"/>
+      <c r="G30" s="18"/>
+      <c r="H30" s="18"/>
+      <c r="I30" s="18"/>
+      <c r="J30" s="18"/>
+      <c r="K30" s="18"/>
+      <c r="L30" s="18"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="18"/>
+      <c r="O30" s="18"/>
+      <c r="P30" s="18"/>
+      <c r="Q30" s="18"/>
+      <c r="R30" s="18"/>
+      <c r="S30" s="18"/>
+      <c r="T30" s="18"/>
+      <c r="U30" s="18"/>
+      <c r="V30" s="18"/>
+      <c r="W30" s="18"/>
+      <c r="X30" s="18"/>
+      <c r="Y30" s="18"/>
+      <c r="Z30" s="27"/>
+      <c r="AA30" s="27"/>
+      <c r="AB30" s="27"/>
+      <c r="AC30" s="27"/>
+      <c r="AD30" s="27"/>
+      <c r="AE30" s="27"/>
+      <c r="AF30" s="27"/>
+      <c r="AG30" s="27"/>
+      <c r="AH30" s="27"/>
+      <c r="AI30" s="27"/>
+      <c r="AJ30" s="27"/>
+      <c r="AK30" s="27"/>
+      <c r="AL30" s="28"/>
       <c r="AM30" s="1"/>
       <c r="AN30" s="1"/>
       <c r="AO30" s="1"/>
@@ -2600,50 +2600,50 @@
       <c r="AR30" s="1"/>
     </row>
     <row r="31" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="38">
+      <c r="A31" s="29">
         <v>26</v>
       </c>
-      <c r="B31" s="39" t="s">
+      <c r="B31" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="40" t="s">
+      <c r="C31" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="D31" s="40"/>
-      <c r="E31" s="40"/>
-      <c r="F31" s="40"/>
-      <c r="G31" s="40"/>
-      <c r="H31" s="40"/>
-      <c r="I31" s="40"/>
-      <c r="J31" s="40"/>
-      <c r="K31" s="40"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="40"/>
-      <c r="N31" s="40"/>
-      <c r="O31" s="40"/>
-      <c r="P31" s="40"/>
-      <c r="Q31" s="40"/>
-      <c r="R31" s="40"/>
-      <c r="S31" s="40"/>
-      <c r="T31" s="40"/>
-      <c r="U31" s="40"/>
-      <c r="V31" s="40"/>
-      <c r="W31" s="40"/>
-      <c r="X31" s="40"/>
-      <c r="Y31" s="40"/>
-      <c r="Z31" s="40"/>
-      <c r="AA31" s="40"/>
-      <c r="AB31" s="40"/>
-      <c r="AC31" s="40"/>
-      <c r="AD31" s="40"/>
-      <c r="AE31" s="40"/>
-      <c r="AF31" s="40"/>
-      <c r="AG31" s="40"/>
-      <c r="AH31" s="40"/>
-      <c r="AI31" s="40"/>
-      <c r="AJ31" s="40"/>
-      <c r="AK31" s="40"/>
-      <c r="AL31" s="41"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
+      <c r="H31" s="31"/>
+      <c r="I31" s="31"/>
+      <c r="J31" s="31"/>
+      <c r="K31" s="31"/>
+      <c r="L31" s="31"/>
+      <c r="M31" s="31"/>
+      <c r="N31" s="31"/>
+      <c r="O31" s="31"/>
+      <c r="P31" s="31"/>
+      <c r="Q31" s="31"/>
+      <c r="R31" s="31"/>
+      <c r="S31" s="31"/>
+      <c r="T31" s="31"/>
+      <c r="U31" s="31"/>
+      <c r="V31" s="31"/>
+      <c r="W31" s="31"/>
+      <c r="X31" s="31"/>
+      <c r="Y31" s="31"/>
+      <c r="Z31" s="31"/>
+      <c r="AA31" s="31"/>
+      <c r="AB31" s="31"/>
+      <c r="AC31" s="31"/>
+      <c r="AD31" s="31"/>
+      <c r="AE31" s="31"/>
+      <c r="AF31" s="31"/>
+      <c r="AG31" s="31"/>
+      <c r="AH31" s="31"/>
+      <c r="AI31" s="31"/>
+      <c r="AJ31" s="31"/>
+      <c r="AK31" s="31"/>
+      <c r="AL31" s="32"/>
       <c r="AM31" s="1"/>
       <c r="AN31" s="1"/>
       <c r="AO31" s="1"/>
@@ -2744,43 +2744,43 @@
       <c r="B34" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="57" t="s">
+      <c r="D34" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="58"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
-      <c r="J34" s="58"/>
-      <c r="K34" s="58"/>
-      <c r="L34" s="58"/>
-      <c r="M34" s="58"/>
-      <c r="N34" s="58"/>
-      <c r="O34" s="58"/>
-      <c r="P34" s="58"/>
-      <c r="Q34" s="58"/>
-      <c r="R34" s="58"/>
-      <c r="S34" s="58"/>
-      <c r="T34" s="58"/>
-      <c r="U34" s="58"/>
-      <c r="V34" s="58"/>
-      <c r="W34" s="58"/>
-      <c r="X34" s="58"/>
-      <c r="Y34" s="58"/>
-      <c r="Z34" s="58"/>
-      <c r="AA34" s="58"/>
-      <c r="AB34" s="58"/>
-      <c r="AC34" s="58"/>
-      <c r="AD34" s="58"/>
-      <c r="AE34" s="58"/>
-      <c r="AF34" s="58"/>
-      <c r="AG34" s="58"/>
-      <c r="AH34" s="58"/>
-      <c r="AI34" s="58"/>
-      <c r="AJ34" s="58"/>
-      <c r="AK34" s="58"/>
-      <c r="AL34" s="59"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="49"/>
+      <c r="V34" s="49"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="49"/>
+      <c r="Y34" s="49"/>
+      <c r="Z34" s="49"/>
+      <c r="AA34" s="49"/>
+      <c r="AB34" s="49"/>
+      <c r="AC34" s="49"/>
+      <c r="AD34" s="49"/>
+      <c r="AE34" s="49"/>
+      <c r="AF34" s="49"/>
+      <c r="AG34" s="49"/>
+      <c r="AH34" s="49"/>
+      <c r="AI34" s="49"/>
+      <c r="AJ34" s="49"/>
+      <c r="AK34" s="49"/>
+      <c r="AL34" s="50"/>
     </row>
     <row r="35" spans="1:44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
@@ -2828,41 +2828,41 @@
       <c r="B36" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="48"/>
-      <c r="E36" s="49"/>
-      <c r="F36" s="49"/>
-      <c r="G36" s="49"/>
-      <c r="H36" s="49"/>
-      <c r="I36" s="49"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="49"/>
-      <c r="L36" s="49"/>
-      <c r="M36" s="49"/>
-      <c r="N36" s="49"/>
-      <c r="O36" s="49"/>
-      <c r="P36" s="49"/>
-      <c r="Q36" s="49"/>
-      <c r="R36" s="49"/>
-      <c r="S36" s="49"/>
-      <c r="T36" s="49"/>
-      <c r="U36" s="49"/>
-      <c r="V36" s="49"/>
-      <c r="W36" s="49"/>
-      <c r="X36" s="49"/>
-      <c r="Y36" s="49"/>
-      <c r="Z36" s="49"/>
-      <c r="AA36" s="49"/>
-      <c r="AB36" s="49"/>
-      <c r="AC36" s="49"/>
-      <c r="AD36" s="49"/>
-      <c r="AE36" s="49"/>
-      <c r="AF36" s="49"/>
-      <c r="AG36" s="49"/>
-      <c r="AH36" s="49"/>
-      <c r="AI36" s="49"/>
-      <c r="AJ36" s="49"/>
-      <c r="AK36" s="49"/>
-      <c r="AL36" s="50"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="55"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="55"/>
+      <c r="T36" s="55"/>
+      <c r="U36" s="55"/>
+      <c r="V36" s="55"/>
+      <c r="W36" s="55"/>
+      <c r="X36" s="55"/>
+      <c r="Y36" s="55"/>
+      <c r="Z36" s="55"/>
+      <c r="AA36" s="55"/>
+      <c r="AB36" s="55"/>
+      <c r="AC36" s="55"/>
+      <c r="AD36" s="55"/>
+      <c r="AE36" s="55"/>
+      <c r="AF36" s="55"/>
+      <c r="AG36" s="55"/>
+      <c r="AH36" s="55"/>
+      <c r="AI36" s="55"/>
+      <c r="AJ36" s="55"/>
+      <c r="AK36" s="55"/>
+      <c r="AL36" s="56"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
       <c r="AP36" s="1"/>
@@ -2870,45 +2870,45 @@
       <c r="AR36" s="1"/>
     </row>
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="44"/>
-      <c r="B37" s="43" t="s">
+      <c r="A37" s="35"/>
+      <c r="B37" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="54"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="55"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="55"/>
-      <c r="I37" s="55"/>
-      <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="55"/>
-      <c r="M37" s="55"/>
-      <c r="N37" s="55"/>
-      <c r="O37" s="55"/>
-      <c r="P37" s="55"/>
-      <c r="Q37" s="55"/>
-      <c r="R37" s="55"/>
-      <c r="S37" s="55"/>
-      <c r="T37" s="55"/>
-      <c r="U37" s="55"/>
-      <c r="V37" s="55"/>
-      <c r="W37" s="55"/>
-      <c r="X37" s="55"/>
-      <c r="Y37" s="55"/>
-      <c r="Z37" s="55"/>
-      <c r="AA37" s="55"/>
-      <c r="AB37" s="55"/>
-      <c r="AC37" s="55"/>
-      <c r="AD37" s="55"/>
-      <c r="AE37" s="55"/>
-      <c r="AF37" s="55"/>
-      <c r="AG37" s="55"/>
-      <c r="AH37" s="55"/>
-      <c r="AI37" s="55"/>
-      <c r="AJ37" s="55"/>
-      <c r="AK37" s="55"/>
-      <c r="AL37" s="56"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="58"/>
+      <c r="T37" s="58"/>
+      <c r="U37" s="58"/>
+      <c r="V37" s="58"/>
+      <c r="W37" s="58"/>
+      <c r="X37" s="58"/>
+      <c r="Y37" s="58"/>
+      <c r="Z37" s="58"/>
+      <c r="AA37" s="58"/>
+      <c r="AB37" s="58"/>
+      <c r="AC37" s="58"/>
+      <c r="AD37" s="58"/>
+      <c r="AE37" s="58"/>
+      <c r="AF37" s="58"/>
+      <c r="AG37" s="58"/>
+      <c r="AH37" s="58"/>
+      <c r="AI37" s="58"/>
+      <c r="AJ37" s="58"/>
+      <c r="AK37" s="58"/>
+      <c r="AL37" s="59"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
     </row>

</xml_diff>

<commit_message>
Actualizados documentos de planeación
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -596,6 +596,33 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,33 +650,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,7 +973,7 @@
   <dimension ref="A1:AR51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="W5" sqref="W1:W1048576"/>
+      <selection activeCell="W19" sqref="W19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,46 +988,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -1036,44 +1036,44 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
@@ -1082,52 +1082,52 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="54"/>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="54"/>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="54"/>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="54"/>
-      <c r="AL3" s="55"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="40"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
@@ -1136,48 +1136,48 @@
       <c r="AR3" s="1"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="58"/>
-      <c r="AC4" s="58"/>
-      <c r="AD4" s="58"/>
-      <c r="AE4" s="58"/>
-      <c r="AF4" s="58"/>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="58"/>
-      <c r="AJ4" s="58"/>
-      <c r="AK4" s="58"/>
-      <c r="AL4" s="59"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
+      <c r="AG4" s="43"/>
+      <c r="AH4" s="43"/>
+      <c r="AI4" s="43"/>
+      <c r="AJ4" s="43"/>
+      <c r="AK4" s="43"/>
+      <c r="AL4" s="44"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
@@ -1186,9 +1186,9 @@
       <c r="AR4" s="1"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="11">
         <v>17</v>
       </c>
@@ -1794,7 +1794,7 @@
       <c r="P15" s="16"/>
       <c r="Q15" s="24"/>
       <c r="R15" s="24"/>
-      <c r="S15" s="17"/>
+      <c r="S15" s="24"/>
       <c r="T15" s="17"/>
       <c r="U15" s="18"/>
       <c r="V15" s="18"/>
@@ -1846,7 +1846,7 @@
       <c r="P16" s="16"/>
       <c r="Q16" s="24"/>
       <c r="R16" s="24"/>
-      <c r="S16" s="17"/>
+      <c r="S16" s="24"/>
       <c r="T16" s="17"/>
       <c r="U16" s="18"/>
       <c r="V16" s="18"/>
@@ -2701,168 +2701,168 @@
       <c r="B33" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="37"/>
-      <c r="S33" s="37"/>
-      <c r="T33" s="37"/>
-      <c r="U33" s="37"/>
-      <c r="V33" s="37"/>
-      <c r="W33" s="37"/>
-      <c r="X33" s="37"/>
-      <c r="Y33" s="37"/>
-      <c r="Z33" s="37"/>
-      <c r="AA33" s="37"/>
-      <c r="AB33" s="37"/>
-      <c r="AC33" s="37"/>
-      <c r="AD33" s="37"/>
-      <c r="AE33" s="37"/>
-      <c r="AF33" s="37"/>
-      <c r="AG33" s="37"/>
-      <c r="AH33" s="37"/>
-      <c r="AI33" s="37"/>
-      <c r="AJ33" s="37"/>
-      <c r="AK33" s="37"/>
-      <c r="AL33" s="38"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="46"/>
+      <c r="V33" s="46"/>
+      <c r="W33" s="46"/>
+      <c r="X33" s="46"/>
+      <c r="Y33" s="46"/>
+      <c r="Z33" s="46"/>
+      <c r="AA33" s="46"/>
+      <c r="AB33" s="46"/>
+      <c r="AC33" s="46"/>
+      <c r="AD33" s="46"/>
+      <c r="AE33" s="46"/>
+      <c r="AF33" s="46"/>
+      <c r="AG33" s="46"/>
+      <c r="AH33" s="46"/>
+      <c r="AI33" s="46"/>
+      <c r="AJ33" s="46"/>
+      <c r="AK33" s="46"/>
+      <c r="AL33" s="47"/>
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D34" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="40"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-      <c r="O34" s="40"/>
-      <c r="P34" s="40"/>
-      <c r="Q34" s="40"/>
-      <c r="R34" s="40"/>
-      <c r="S34" s="40"/>
-      <c r="T34" s="40"/>
-      <c r="U34" s="40"/>
-      <c r="V34" s="40"/>
-      <c r="W34" s="40"/>
-      <c r="X34" s="40"/>
-      <c r="Y34" s="40"/>
-      <c r="Z34" s="40"/>
-      <c r="AA34" s="40"/>
-      <c r="AB34" s="40"/>
-      <c r="AC34" s="40"/>
-      <c r="AD34" s="40"/>
-      <c r="AE34" s="40"/>
-      <c r="AF34" s="40"/>
-      <c r="AG34" s="40"/>
-      <c r="AH34" s="40"/>
-      <c r="AI34" s="40"/>
-      <c r="AJ34" s="40"/>
-      <c r="AK34" s="40"/>
-      <c r="AL34" s="41"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="49"/>
+      <c r="V34" s="49"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="49"/>
+      <c r="Y34" s="49"/>
+      <c r="Z34" s="49"/>
+      <c r="AA34" s="49"/>
+      <c r="AB34" s="49"/>
+      <c r="AC34" s="49"/>
+      <c r="AD34" s="49"/>
+      <c r="AE34" s="49"/>
+      <c r="AF34" s="49"/>
+      <c r="AG34" s="49"/>
+      <c r="AH34" s="49"/>
+      <c r="AI34" s="49"/>
+      <c r="AJ34" s="49"/>
+      <c r="AK34" s="49"/>
+      <c r="AL34" s="50"/>
     </row>
     <row r="35" spans="1:44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="43"/>
-      <c r="R35" s="43"/>
-      <c r="S35" s="43"/>
-      <c r="T35" s="43"/>
-      <c r="U35" s="43"/>
-      <c r="V35" s="43"/>
-      <c r="W35" s="43"/>
-      <c r="X35" s="43"/>
-      <c r="Y35" s="43"/>
-      <c r="Z35" s="43"/>
-      <c r="AA35" s="43"/>
-      <c r="AB35" s="43"/>
-      <c r="AC35" s="43"/>
-      <c r="AD35" s="43"/>
-      <c r="AE35" s="43"/>
-      <c r="AF35" s="43"/>
-      <c r="AG35" s="43"/>
-      <c r="AH35" s="43"/>
-      <c r="AI35" s="43"/>
-      <c r="AJ35" s="43"/>
-      <c r="AK35" s="43"/>
-      <c r="AL35" s="44"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="52"/>
+      <c r="R35" s="52"/>
+      <c r="S35" s="52"/>
+      <c r="T35" s="52"/>
+      <c r="U35" s="52"/>
+      <c r="V35" s="52"/>
+      <c r="W35" s="52"/>
+      <c r="X35" s="52"/>
+      <c r="Y35" s="52"/>
+      <c r="Z35" s="52"/>
+      <c r="AA35" s="52"/>
+      <c r="AB35" s="52"/>
+      <c r="AC35" s="52"/>
+      <c r="AD35" s="52"/>
+      <c r="AE35" s="52"/>
+      <c r="AF35" s="52"/>
+      <c r="AG35" s="52"/>
+      <c r="AH35" s="52"/>
+      <c r="AI35" s="52"/>
+      <c r="AJ35" s="52"/>
+      <c r="AK35" s="52"/>
+      <c r="AL35" s="53"/>
     </row>
     <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="45"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="46"/>
-      <c r="N36" s="46"/>
-      <c r="O36" s="46"/>
-      <c r="P36" s="46"/>
-      <c r="Q36" s="46"/>
-      <c r="R36" s="46"/>
-      <c r="S36" s="46"/>
-      <c r="T36" s="46"/>
-      <c r="U36" s="46"/>
-      <c r="V36" s="46"/>
-      <c r="W36" s="46"/>
-      <c r="X36" s="46"/>
-      <c r="Y36" s="46"/>
-      <c r="Z36" s="46"/>
-      <c r="AA36" s="46"/>
-      <c r="AB36" s="46"/>
-      <c r="AC36" s="46"/>
-      <c r="AD36" s="46"/>
-      <c r="AE36" s="46"/>
-      <c r="AF36" s="46"/>
-      <c r="AG36" s="46"/>
-      <c r="AH36" s="46"/>
-      <c r="AI36" s="46"/>
-      <c r="AJ36" s="46"/>
-      <c r="AK36" s="46"/>
-      <c r="AL36" s="47"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="55"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="55"/>
+      <c r="T36" s="55"/>
+      <c r="U36" s="55"/>
+      <c r="V36" s="55"/>
+      <c r="W36" s="55"/>
+      <c r="X36" s="55"/>
+      <c r="Y36" s="55"/>
+      <c r="Z36" s="55"/>
+      <c r="AA36" s="55"/>
+      <c r="AB36" s="55"/>
+      <c r="AC36" s="55"/>
+      <c r="AD36" s="55"/>
+      <c r="AE36" s="55"/>
+      <c r="AF36" s="55"/>
+      <c r="AG36" s="55"/>
+      <c r="AH36" s="55"/>
+      <c r="AI36" s="55"/>
+      <c r="AJ36" s="55"/>
+      <c r="AK36" s="55"/>
+      <c r="AL36" s="56"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
       <c r="AP36" s="1"/>
@@ -2874,41 +2874,41 @@
       <c r="B37" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="48"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="49"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="49"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="49"/>
-      <c r="V37" s="49"/>
-      <c r="W37" s="49"/>
-      <c r="X37" s="49"/>
-      <c r="Y37" s="49"/>
-      <c r="Z37" s="49"/>
-      <c r="AA37" s="49"/>
-      <c r="AB37" s="49"/>
-      <c r="AC37" s="49"/>
-      <c r="AD37" s="49"/>
-      <c r="AE37" s="49"/>
-      <c r="AF37" s="49"/>
-      <c r="AG37" s="49"/>
-      <c r="AH37" s="49"/>
-      <c r="AI37" s="49"/>
-      <c r="AJ37" s="49"/>
-      <c r="AK37" s="49"/>
-      <c r="AL37" s="50"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="58"/>
+      <c r="T37" s="58"/>
+      <c r="U37" s="58"/>
+      <c r="V37" s="58"/>
+      <c r="W37" s="58"/>
+      <c r="X37" s="58"/>
+      <c r="Y37" s="58"/>
+      <c r="Z37" s="58"/>
+      <c r="AA37" s="58"/>
+      <c r="AB37" s="58"/>
+      <c r="AC37" s="58"/>
+      <c r="AD37" s="58"/>
+      <c r="AE37" s="58"/>
+      <c r="AF37" s="58"/>
+      <c r="AG37" s="58"/>
+      <c r="AH37" s="58"/>
+      <c r="AI37" s="58"/>
+      <c r="AJ37" s="58"/>
+      <c r="AK37" s="58"/>
+      <c r="AL37" s="59"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
     </row>
@@ -3401,6 +3401,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D33:AL33"/>
+    <mergeCell ref="D34:AL34"/>
+    <mergeCell ref="D35:AL35"/>
+    <mergeCell ref="D36:AL36"/>
+    <mergeCell ref="D37:AL37"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A1:AL2"/>
     <mergeCell ref="D3:AL3"/>
@@ -3408,11 +3413,6 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D4:R4"/>
     <mergeCell ref="S4:AL4"/>
-    <mergeCell ref="D33:AL33"/>
-    <mergeCell ref="D34:AL34"/>
-    <mergeCell ref="D35:AL35"/>
-    <mergeCell ref="D36:AL36"/>
-    <mergeCell ref="D37:AL37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Parche para resolver Issue #7
-Ahora el juego te muestra si ganaste la ronda o no, y por qué.
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -596,6 +596,33 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -623,33 +650,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,7 +973,7 @@
   <dimension ref="A1:AR51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AI17" sqref="AI17"/>
+      <selection activeCell="AN19" sqref="AN19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -988,46 +988,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
-      <c r="F1" s="53"/>
-      <c r="G1" s="53"/>
-      <c r="H1" s="53"/>
-      <c r="I1" s="53"/>
-      <c r="J1" s="53"/>
-      <c r="K1" s="53"/>
-      <c r="L1" s="53"/>
-      <c r="M1" s="53"/>
-      <c r="N1" s="53"/>
-      <c r="O1" s="53"/>
-      <c r="P1" s="53"/>
-      <c r="Q1" s="53"/>
-      <c r="R1" s="53"/>
-      <c r="S1" s="53"/>
-      <c r="T1" s="53"/>
-      <c r="U1" s="53"/>
-      <c r="V1" s="53"/>
-      <c r="W1" s="53"/>
-      <c r="X1" s="53"/>
-      <c r="Y1" s="53"/>
-      <c r="Z1" s="53"/>
-      <c r="AA1" s="53"/>
-      <c r="AB1" s="53"/>
-      <c r="AC1" s="53"/>
-      <c r="AD1" s="53"/>
-      <c r="AE1" s="53"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="53"/>
-      <c r="AJ1" s="53"/>
-      <c r="AK1" s="53"/>
-      <c r="AL1" s="53"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="38"/>
+      <c r="J1" s="38"/>
+      <c r="K1" s="38"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="38"/>
+      <c r="N1" s="38"/>
+      <c r="O1" s="38"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="38"/>
+      <c r="R1" s="38"/>
+      <c r="S1" s="38"/>
+      <c r="T1" s="38"/>
+      <c r="U1" s="38"/>
+      <c r="V1" s="38"/>
+      <c r="W1" s="38"/>
+      <c r="X1" s="38"/>
+      <c r="Y1" s="38"/>
+      <c r="Z1" s="38"/>
+      <c r="AA1" s="38"/>
+      <c r="AB1" s="38"/>
+      <c r="AC1" s="38"/>
+      <c r="AD1" s="38"/>
+      <c r="AE1" s="38"/>
+      <c r="AF1" s="38"/>
+      <c r="AG1" s="38"/>
+      <c r="AH1" s="38"/>
+      <c r="AI1" s="38"/>
+      <c r="AJ1" s="38"/>
+      <c r="AK1" s="38"/>
+      <c r="AL1" s="38"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -1036,44 +1036,44 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="53"/>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="53"/>
-      <c r="E2" s="53"/>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="53"/>
-      <c r="I2" s="53"/>
-      <c r="J2" s="53"/>
-      <c r="K2" s="53"/>
-      <c r="L2" s="53"/>
-      <c r="M2" s="53"/>
-      <c r="N2" s="53"/>
-      <c r="O2" s="53"/>
-      <c r="P2" s="53"/>
-      <c r="Q2" s="53"/>
-      <c r="R2" s="53"/>
-      <c r="S2" s="53"/>
-      <c r="T2" s="53"/>
-      <c r="U2" s="53"/>
-      <c r="V2" s="53"/>
-      <c r="W2" s="53"/>
-      <c r="X2" s="53"/>
-      <c r="Y2" s="53"/>
-      <c r="Z2" s="53"/>
-      <c r="AA2" s="53"/>
-      <c r="AB2" s="53"/>
-      <c r="AC2" s="53"/>
-      <c r="AD2" s="53"/>
-      <c r="AE2" s="53"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="53"/>
-      <c r="AJ2" s="53"/>
-      <c r="AK2" s="53"/>
-      <c r="AL2" s="53"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="38"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="38"/>
+      <c r="J2" s="38"/>
+      <c r="K2" s="38"/>
+      <c r="L2" s="38"/>
+      <c r="M2" s="38"/>
+      <c r="N2" s="38"/>
+      <c r="O2" s="38"/>
+      <c r="P2" s="38"/>
+      <c r="Q2" s="38"/>
+      <c r="R2" s="38"/>
+      <c r="S2" s="38"/>
+      <c r="T2" s="38"/>
+      <c r="U2" s="38"/>
+      <c r="V2" s="38"/>
+      <c r="W2" s="38"/>
+      <c r="X2" s="38"/>
+      <c r="Y2" s="38"/>
+      <c r="Z2" s="38"/>
+      <c r="AA2" s="38"/>
+      <c r="AB2" s="38"/>
+      <c r="AC2" s="38"/>
+      <c r="AD2" s="38"/>
+      <c r="AE2" s="38"/>
+      <c r="AF2" s="38"/>
+      <c r="AG2" s="38"/>
+      <c r="AH2" s="38"/>
+      <c r="AI2" s="38"/>
+      <c r="AJ2" s="38"/>
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
@@ -1082,52 +1082,52 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="B3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="56" t="s">
+      <c r="C3" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="54" t="s">
+      <c r="D3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
-      <c r="G3" s="54"/>
-      <c r="H3" s="54"/>
-      <c r="I3" s="54"/>
-      <c r="J3" s="54"/>
-      <c r="K3" s="54"/>
-      <c r="L3" s="54"/>
-      <c r="M3" s="54"/>
-      <c r="N3" s="54"/>
-      <c r="O3" s="54"/>
-      <c r="P3" s="54"/>
-      <c r="Q3" s="54"/>
-      <c r="R3" s="54"/>
-      <c r="S3" s="54"/>
-      <c r="T3" s="54"/>
-      <c r="U3" s="54"/>
-      <c r="V3" s="54"/>
-      <c r="W3" s="54"/>
-      <c r="X3" s="54"/>
-      <c r="Y3" s="54"/>
-      <c r="Z3" s="54"/>
-      <c r="AA3" s="54"/>
-      <c r="AB3" s="54"/>
-      <c r="AC3" s="54"/>
-      <c r="AD3" s="54"/>
-      <c r="AE3" s="54"/>
-      <c r="AF3" s="54"/>
-      <c r="AG3" s="54"/>
-      <c r="AH3" s="54"/>
-      <c r="AI3" s="54"/>
-      <c r="AJ3" s="54"/>
-      <c r="AK3" s="54"/>
-      <c r="AL3" s="55"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="39"/>
+      <c r="V3" s="39"/>
+      <c r="W3" s="39"/>
+      <c r="X3" s="39"/>
+      <c r="Y3" s="39"/>
+      <c r="Z3" s="39"/>
+      <c r="AA3" s="39"/>
+      <c r="AB3" s="39"/>
+      <c r="AC3" s="39"/>
+      <c r="AD3" s="39"/>
+      <c r="AE3" s="39"/>
+      <c r="AF3" s="39"/>
+      <c r="AG3" s="39"/>
+      <c r="AH3" s="39"/>
+      <c r="AI3" s="39"/>
+      <c r="AJ3" s="39"/>
+      <c r="AK3" s="39"/>
+      <c r="AL3" s="40"/>
       <c r="AM3" s="1"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
@@ -1136,48 +1136,48 @@
       <c r="AR3" s="1"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="52"/>
-      <c r="B4" s="57"/>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58" t="s">
+      <c r="A4" s="37"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="43" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="58"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="58"/>
-      <c r="I4" s="58"/>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58"/>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58" t="s">
+      <c r="E4" s="43"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="43"/>
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43"/>
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="58"/>
-      <c r="X4" s="58"/>
-      <c r="Y4" s="58"/>
-      <c r="Z4" s="58"/>
-      <c r="AA4" s="58"/>
-      <c r="AB4" s="58"/>
-      <c r="AC4" s="58"/>
-      <c r="AD4" s="58"/>
-      <c r="AE4" s="58"/>
-      <c r="AF4" s="58"/>
-      <c r="AG4" s="58"/>
-      <c r="AH4" s="58"/>
-      <c r="AI4" s="58"/>
-      <c r="AJ4" s="58"/>
-      <c r="AK4" s="58"/>
-      <c r="AL4" s="59"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="43"/>
+      <c r="Y4" s="43"/>
+      <c r="Z4" s="43"/>
+      <c r="AA4" s="43"/>
+      <c r="AB4" s="43"/>
+      <c r="AC4" s="43"/>
+      <c r="AD4" s="43"/>
+      <c r="AE4" s="43"/>
+      <c r="AF4" s="43"/>
+      <c r="AG4" s="43"/>
+      <c r="AH4" s="43"/>
+      <c r="AI4" s="43"/>
+      <c r="AJ4" s="43"/>
+      <c r="AK4" s="43"/>
+      <c r="AL4" s="44"/>
       <c r="AM4" s="1"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
@@ -1186,9 +1186,9 @@
       <c r="AR4" s="1"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="52"/>
-      <c r="B5" s="57"/>
-      <c r="C5" s="57"/>
+      <c r="A5" s="37"/>
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
       <c r="D5" s="11">
         <v>17</v>
       </c>
@@ -2274,11 +2274,11 @@
       <c r="AD24" s="16"/>
       <c r="AE24" s="16"/>
       <c r="AF24" s="16"/>
-      <c r="AG24" s="18"/>
-      <c r="AH24" s="18"/>
-      <c r="AI24" s="18"/>
-      <c r="AJ24" s="18"/>
-      <c r="AK24" s="18"/>
+      <c r="AG24" s="16"/>
+      <c r="AH24" s="16"/>
+      <c r="AI24" s="16"/>
+      <c r="AJ24" s="16"/>
+      <c r="AK24" s="16"/>
       <c r="AL24" s="19"/>
       <c r="AM24" s="1"/>
       <c r="AN24" s="1"/>
@@ -2701,168 +2701,168 @@
       <c r="B33" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="36" t="s">
+      <c r="D33" s="45" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="37"/>
-      <c r="F33" s="37"/>
-      <c r="G33" s="37"/>
-      <c r="H33" s="37"/>
-      <c r="I33" s="37"/>
-      <c r="J33" s="37"/>
-      <c r="K33" s="37"/>
-      <c r="L33" s="37"/>
-      <c r="M33" s="37"/>
-      <c r="N33" s="37"/>
-      <c r="O33" s="37"/>
-      <c r="P33" s="37"/>
-      <c r="Q33" s="37"/>
-      <c r="R33" s="37"/>
-      <c r="S33" s="37"/>
-      <c r="T33" s="37"/>
-      <c r="U33" s="37"/>
-      <c r="V33" s="37"/>
-      <c r="W33" s="37"/>
-      <c r="X33" s="37"/>
-      <c r="Y33" s="37"/>
-      <c r="Z33" s="37"/>
-      <c r="AA33" s="37"/>
-      <c r="AB33" s="37"/>
-      <c r="AC33" s="37"/>
-      <c r="AD33" s="37"/>
-      <c r="AE33" s="37"/>
-      <c r="AF33" s="37"/>
-      <c r="AG33" s="37"/>
-      <c r="AH33" s="37"/>
-      <c r="AI33" s="37"/>
-      <c r="AJ33" s="37"/>
-      <c r="AK33" s="37"/>
-      <c r="AL33" s="38"/>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
+      <c r="J33" s="46"/>
+      <c r="K33" s="46"/>
+      <c r="L33" s="46"/>
+      <c r="M33" s="46"/>
+      <c r="N33" s="46"/>
+      <c r="O33" s="46"/>
+      <c r="P33" s="46"/>
+      <c r="Q33" s="46"/>
+      <c r="R33" s="46"/>
+      <c r="S33" s="46"/>
+      <c r="T33" s="46"/>
+      <c r="U33" s="46"/>
+      <c r="V33" s="46"/>
+      <c r="W33" s="46"/>
+      <c r="X33" s="46"/>
+      <c r="Y33" s="46"/>
+      <c r="Z33" s="46"/>
+      <c r="AA33" s="46"/>
+      <c r="AB33" s="46"/>
+      <c r="AC33" s="46"/>
+      <c r="AD33" s="46"/>
+      <c r="AE33" s="46"/>
+      <c r="AF33" s="46"/>
+      <c r="AG33" s="46"/>
+      <c r="AH33" s="46"/>
+      <c r="AI33" s="46"/>
+      <c r="AJ33" s="46"/>
+      <c r="AK33" s="46"/>
+      <c r="AL33" s="47"/>
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="39" t="s">
+      <c r="D34" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="40"/>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="40"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="40"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="40"/>
-      <c r="N34" s="40"/>
-      <c r="O34" s="40"/>
-      <c r="P34" s="40"/>
-      <c r="Q34" s="40"/>
-      <c r="R34" s="40"/>
-      <c r="S34" s="40"/>
-      <c r="T34" s="40"/>
-      <c r="U34" s="40"/>
-      <c r="V34" s="40"/>
-      <c r="W34" s="40"/>
-      <c r="X34" s="40"/>
-      <c r="Y34" s="40"/>
-      <c r="Z34" s="40"/>
-      <c r="AA34" s="40"/>
-      <c r="AB34" s="40"/>
-      <c r="AC34" s="40"/>
-      <c r="AD34" s="40"/>
-      <c r="AE34" s="40"/>
-      <c r="AF34" s="40"/>
-      <c r="AG34" s="40"/>
-      <c r="AH34" s="40"/>
-      <c r="AI34" s="40"/>
-      <c r="AJ34" s="40"/>
-      <c r="AK34" s="40"/>
-      <c r="AL34" s="41"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
+      <c r="M34" s="49"/>
+      <c r="N34" s="49"/>
+      <c r="O34" s="49"/>
+      <c r="P34" s="49"/>
+      <c r="Q34" s="49"/>
+      <c r="R34" s="49"/>
+      <c r="S34" s="49"/>
+      <c r="T34" s="49"/>
+      <c r="U34" s="49"/>
+      <c r="V34" s="49"/>
+      <c r="W34" s="49"/>
+      <c r="X34" s="49"/>
+      <c r="Y34" s="49"/>
+      <c r="Z34" s="49"/>
+      <c r="AA34" s="49"/>
+      <c r="AB34" s="49"/>
+      <c r="AC34" s="49"/>
+      <c r="AD34" s="49"/>
+      <c r="AE34" s="49"/>
+      <c r="AF34" s="49"/>
+      <c r="AG34" s="49"/>
+      <c r="AH34" s="49"/>
+      <c r="AI34" s="49"/>
+      <c r="AJ34" s="49"/>
+      <c r="AK34" s="49"/>
+      <c r="AL34" s="50"/>
     </row>
     <row r="35" spans="1:44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="42"/>
-      <c r="E35" s="43"/>
-      <c r="F35" s="43"/>
-      <c r="G35" s="43"/>
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
-      <c r="K35" s="43"/>
-      <c r="L35" s="43"/>
-      <c r="M35" s="43"/>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
-      <c r="P35" s="43"/>
-      <c r="Q35" s="43"/>
-      <c r="R35" s="43"/>
-      <c r="S35" s="43"/>
-      <c r="T35" s="43"/>
-      <c r="U35" s="43"/>
-      <c r="V35" s="43"/>
-      <c r="W35" s="43"/>
-      <c r="X35" s="43"/>
-      <c r="Y35" s="43"/>
-      <c r="Z35" s="43"/>
-      <c r="AA35" s="43"/>
-      <c r="AB35" s="43"/>
-      <c r="AC35" s="43"/>
-      <c r="AD35" s="43"/>
-      <c r="AE35" s="43"/>
-      <c r="AF35" s="43"/>
-      <c r="AG35" s="43"/>
-      <c r="AH35" s="43"/>
-      <c r="AI35" s="43"/>
-      <c r="AJ35" s="43"/>
-      <c r="AK35" s="43"/>
-      <c r="AL35" s="44"/>
+      <c r="D35" s="51"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="52"/>
+      <c r="H35" s="52"/>
+      <c r="I35" s="52"/>
+      <c r="J35" s="52"/>
+      <c r="K35" s="52"/>
+      <c r="L35" s="52"/>
+      <c r="M35" s="52"/>
+      <c r="N35" s="52"/>
+      <c r="O35" s="52"/>
+      <c r="P35" s="52"/>
+      <c r="Q35" s="52"/>
+      <c r="R35" s="52"/>
+      <c r="S35" s="52"/>
+      <c r="T35" s="52"/>
+      <c r="U35" s="52"/>
+      <c r="V35" s="52"/>
+      <c r="W35" s="52"/>
+      <c r="X35" s="52"/>
+      <c r="Y35" s="52"/>
+      <c r="Z35" s="52"/>
+      <c r="AA35" s="52"/>
+      <c r="AB35" s="52"/>
+      <c r="AC35" s="52"/>
+      <c r="AD35" s="52"/>
+      <c r="AE35" s="52"/>
+      <c r="AF35" s="52"/>
+      <c r="AG35" s="52"/>
+      <c r="AH35" s="52"/>
+      <c r="AI35" s="52"/>
+      <c r="AJ35" s="52"/>
+      <c r="AK35" s="52"/>
+      <c r="AL35" s="53"/>
     </row>
     <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="45"/>
-      <c r="E36" s="46"/>
-      <c r="F36" s="46"/>
-      <c r="G36" s="46"/>
-      <c r="H36" s="46"/>
-      <c r="I36" s="46"/>
-      <c r="J36" s="46"/>
-      <c r="K36" s="46"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="46"/>
-      <c r="N36" s="46"/>
-      <c r="O36" s="46"/>
-      <c r="P36" s="46"/>
-      <c r="Q36" s="46"/>
-      <c r="R36" s="46"/>
-      <c r="S36" s="46"/>
-      <c r="T36" s="46"/>
-      <c r="U36" s="46"/>
-      <c r="V36" s="46"/>
-      <c r="W36" s="46"/>
-      <c r="X36" s="46"/>
-      <c r="Y36" s="46"/>
-      <c r="Z36" s="46"/>
-      <c r="AA36" s="46"/>
-      <c r="AB36" s="46"/>
-      <c r="AC36" s="46"/>
-      <c r="AD36" s="46"/>
-      <c r="AE36" s="46"/>
-      <c r="AF36" s="46"/>
-      <c r="AG36" s="46"/>
-      <c r="AH36" s="46"/>
-      <c r="AI36" s="46"/>
-      <c r="AJ36" s="46"/>
-      <c r="AK36" s="46"/>
-      <c r="AL36" s="47"/>
+      <c r="D36" s="54"/>
+      <c r="E36" s="55"/>
+      <c r="F36" s="55"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="55"/>
+      <c r="I36" s="55"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="55"/>
+      <c r="M36" s="55"/>
+      <c r="N36" s="55"/>
+      <c r="O36" s="55"/>
+      <c r="P36" s="55"/>
+      <c r="Q36" s="55"/>
+      <c r="R36" s="55"/>
+      <c r="S36" s="55"/>
+      <c r="T36" s="55"/>
+      <c r="U36" s="55"/>
+      <c r="V36" s="55"/>
+      <c r="W36" s="55"/>
+      <c r="X36" s="55"/>
+      <c r="Y36" s="55"/>
+      <c r="Z36" s="55"/>
+      <c r="AA36" s="55"/>
+      <c r="AB36" s="55"/>
+      <c r="AC36" s="55"/>
+      <c r="AD36" s="55"/>
+      <c r="AE36" s="55"/>
+      <c r="AF36" s="55"/>
+      <c r="AG36" s="55"/>
+      <c r="AH36" s="55"/>
+      <c r="AI36" s="55"/>
+      <c r="AJ36" s="55"/>
+      <c r="AK36" s="55"/>
+      <c r="AL36" s="56"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
       <c r="AP36" s="1"/>
@@ -2874,41 +2874,41 @@
       <c r="B37" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="D37" s="48"/>
-      <c r="E37" s="49"/>
-      <c r="F37" s="49"/>
-      <c r="G37" s="49"/>
-      <c r="H37" s="49"/>
-      <c r="I37" s="49"/>
-      <c r="J37" s="49"/>
-      <c r="K37" s="49"/>
-      <c r="L37" s="49"/>
-      <c r="M37" s="49"/>
-      <c r="N37" s="49"/>
-      <c r="O37" s="49"/>
-      <c r="P37" s="49"/>
-      <c r="Q37" s="49"/>
-      <c r="R37" s="49"/>
-      <c r="S37" s="49"/>
-      <c r="T37" s="49"/>
-      <c r="U37" s="49"/>
-      <c r="V37" s="49"/>
-      <c r="W37" s="49"/>
-      <c r="X37" s="49"/>
-      <c r="Y37" s="49"/>
-      <c r="Z37" s="49"/>
-      <c r="AA37" s="49"/>
-      <c r="AB37" s="49"/>
-      <c r="AC37" s="49"/>
-      <c r="AD37" s="49"/>
-      <c r="AE37" s="49"/>
-      <c r="AF37" s="49"/>
-      <c r="AG37" s="49"/>
-      <c r="AH37" s="49"/>
-      <c r="AI37" s="49"/>
-      <c r="AJ37" s="49"/>
-      <c r="AK37" s="49"/>
-      <c r="AL37" s="50"/>
+      <c r="D37" s="57"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="58"/>
+      <c r="G37" s="58"/>
+      <c r="H37" s="58"/>
+      <c r="I37" s="58"/>
+      <c r="J37" s="58"/>
+      <c r="K37" s="58"/>
+      <c r="L37" s="58"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="58"/>
+      <c r="P37" s="58"/>
+      <c r="Q37" s="58"/>
+      <c r="R37" s="58"/>
+      <c r="S37" s="58"/>
+      <c r="T37" s="58"/>
+      <c r="U37" s="58"/>
+      <c r="V37" s="58"/>
+      <c r="W37" s="58"/>
+      <c r="X37" s="58"/>
+      <c r="Y37" s="58"/>
+      <c r="Z37" s="58"/>
+      <c r="AA37" s="58"/>
+      <c r="AB37" s="58"/>
+      <c r="AC37" s="58"/>
+      <c r="AD37" s="58"/>
+      <c r="AE37" s="58"/>
+      <c r="AF37" s="58"/>
+      <c r="AG37" s="58"/>
+      <c r="AH37" s="58"/>
+      <c r="AI37" s="58"/>
+      <c r="AJ37" s="58"/>
+      <c r="AK37" s="58"/>
+      <c r="AL37" s="59"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
     </row>
@@ -3401,6 +3401,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D33:AL33"/>
+    <mergeCell ref="D34:AL34"/>
+    <mergeCell ref="D35:AL35"/>
+    <mergeCell ref="D36:AL36"/>
+    <mergeCell ref="D37:AL37"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A1:AL2"/>
     <mergeCell ref="D3:AL3"/>
@@ -3408,11 +3413,6 @@
     <mergeCell ref="C3:C5"/>
     <mergeCell ref="D4:R4"/>
     <mergeCell ref="S4:AL4"/>
-    <mergeCell ref="D33:AL33"/>
-    <mergeCell ref="D34:AL34"/>
-    <mergeCell ref="D35:AL35"/>
-    <mergeCell ref="D36:AL36"/>
-    <mergeCell ref="D37:AL37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Portada de la caja
-Se creó la portada de la caja del disco.
-Se modificaron las respuestas a los riesgos.
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -72,9 +72,6 @@
     <t>Resolución de Issues</t>
   </si>
   <si>
-    <t>Texturizado de cartas y fichas</t>
-  </si>
-  <si>
     <t>Modelado de cartas y fichas</t>
   </si>
   <si>
@@ -154,6 +151,9 @@
   </si>
   <si>
     <t>"Otros componentes" se refiere a todos los componentes del juego que no son el Cliente, Servidor y Manejador del Juego.</t>
+  </si>
+  <si>
+    <t>Texturizado de objetos</t>
   </si>
 </sst>
 </file>
@@ -972,8 +972,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AN19" sqref="AN19"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AN8" sqref="AN8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="3" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="36" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B3" s="41" t="s">
         <v>2</v>
@@ -1309,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="16"/>
       <c r="E6" s="17"/>
@@ -1413,7 +1413,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D8" s="17"/>
       <c r="E8" s="33"/>
@@ -1517,7 +1517,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" s="17"/>
       <c r="E10" s="16"/>
@@ -1569,7 +1569,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D11" s="17"/>
       <c r="E11" s="16"/>
@@ -1621,7 +1621,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
@@ -1673,7 +1673,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D13" s="18"/>
       <c r="E13" s="18"/>
@@ -1725,7 +1725,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D14" s="18"/>
       <c r="E14" s="18"/>
@@ -1777,7 +1777,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="18"/>
@@ -1829,7 +1829,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="18"/>
@@ -1933,7 +1933,7 @@
         <v>0</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="18"/>
@@ -1985,7 +1985,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D19" s="18"/>
       <c r="E19" s="18"/>
@@ -2037,7 +2037,7 @@
         <v>1</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="18"/>
       <c r="E20" s="18"/>
@@ -2089,7 +2089,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D21" s="18"/>
       <c r="E21" s="18"/>
@@ -2141,7 +2141,7 @@
         <v>0</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D22" s="17"/>
       <c r="E22" s="17"/>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="D23" s="17"/>
       <c r="E23" s="17"/>
@@ -2295,7 +2295,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D25" s="18"/>
       <c r="E25" s="18"/>
@@ -2347,7 +2347,7 @@
         <v>0</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D26" s="18"/>
       <c r="E26" s="18"/>
@@ -2375,7 +2375,7 @@
       <c r="AA26" s="17"/>
       <c r="AB26" s="17"/>
       <c r="AC26" s="22"/>
-      <c r="AD26" s="18"/>
+      <c r="AD26" s="24"/>
       <c r="AE26" s="18"/>
       <c r="AF26" s="18"/>
       <c r="AG26" s="18"/>
@@ -2399,7 +2399,7 @@
         <v>0</v>
       </c>
       <c r="C27" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D27" s="18"/>
       <c r="E27" s="18"/>
@@ -2451,7 +2451,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
@@ -2503,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
@@ -2699,10 +2699,10 @@
     <row r="33" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D33" s="45" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E33" s="46"/>
       <c r="F33" s="46"/>
@@ -2742,10 +2742,10 @@
     <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D34" s="48" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E34" s="49"/>
       <c r="F34" s="49"/>
@@ -2785,7 +2785,7 @@
     <row r="35" spans="1:44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D35" s="51"/>
       <c r="E35" s="52"/>
@@ -2826,7 +2826,7 @@
     <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="54"/>
       <c r="E36" s="55"/>
@@ -2872,7 +2872,7 @@
     <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="35"/>
       <c r="B37" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D37" s="57"/>
       <c r="E37" s="58"/>

</xml_diff>

<commit_message>
Resolución del Issue #14
-El botón que dice "Iniciar prueba" solo se mostrará ahora al ejecutar
el juego desde el editor.
-Se marcó la tarea "Elaboración del instalador" como retrasada. No fue
necesario recalendarizar.
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -596,33 +596,7 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -650,7 +624,33 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -973,8 +973,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AR51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AM12" sqref="AM12"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="AK28" sqref="AK28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,46 +989,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="38"/>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38"/>
-      <c r="J1" s="38"/>
-      <c r="K1" s="38"/>
-      <c r="L1" s="38"/>
-      <c r="M1" s="38"/>
-      <c r="N1" s="38"/>
-      <c r="O1" s="38"/>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="R1" s="38"/>
-      <c r="S1" s="38"/>
-      <c r="T1" s="38"/>
-      <c r="U1" s="38"/>
-      <c r="V1" s="38"/>
-      <c r="W1" s="38"/>
-      <c r="X1" s="38"/>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
-      <c r="AA1" s="38"/>
-      <c r="AB1" s="38"/>
-      <c r="AC1" s="38"/>
-      <c r="AD1" s="38"/>
-      <c r="AE1" s="38"/>
-      <c r="AF1" s="38"/>
-      <c r="AG1" s="38"/>
-      <c r="AH1" s="38"/>
-      <c r="AI1" s="38"/>
-      <c r="AJ1" s="38"/>
-      <c r="AK1" s="38"/>
-      <c r="AL1" s="38"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="54"/>
+      <c r="Q1" s="54"/>
+      <c r="R1" s="54"/>
+      <c r="S1" s="54"/>
+      <c r="T1" s="54"/>
+      <c r="U1" s="54"/>
+      <c r="V1" s="54"/>
+      <c r="W1" s="54"/>
+      <c r="X1" s="54"/>
+      <c r="Y1" s="54"/>
+      <c r="Z1" s="54"/>
+      <c r="AA1" s="54"/>
+      <c r="AB1" s="54"/>
+      <c r="AC1" s="54"/>
+      <c r="AD1" s="54"/>
+      <c r="AE1" s="54"/>
+      <c r="AF1" s="54"/>
+      <c r="AG1" s="54"/>
+      <c r="AH1" s="54"/>
+      <c r="AI1" s="54"/>
+      <c r="AJ1" s="54"/>
+      <c r="AK1" s="54"/>
+      <c r="AL1" s="54"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -1037,44 +1037,44 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="38"/>
-      <c r="B2" s="38"/>
-      <c r="C2" s="38"/>
-      <c r="D2" s="38"/>
-      <c r="E2" s="38"/>
-      <c r="F2" s="38"/>
-      <c r="G2" s="38"/>
-      <c r="H2" s="38"/>
-      <c r="I2" s="38"/>
-      <c r="J2" s="38"/>
-      <c r="K2" s="38"/>
-      <c r="L2" s="38"/>
-      <c r="M2" s="38"/>
-      <c r="N2" s="38"/>
-      <c r="O2" s="38"/>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
-      <c r="Y2" s="38"/>
-      <c r="Z2" s="38"/>
-      <c r="AA2" s="38"/>
-      <c r="AB2" s="38"/>
-      <c r="AC2" s="38"/>
-      <c r="AD2" s="38"/>
-      <c r="AE2" s="38"/>
-      <c r="AF2" s="38"/>
-      <c r="AG2" s="38"/>
-      <c r="AH2" s="38"/>
-      <c r="AI2" s="38"/>
-      <c r="AJ2" s="38"/>
-      <c r="AK2" s="38"/>
-      <c r="AL2" s="38"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="54"/>
+      <c r="J2" s="54"/>
+      <c r="K2" s="54"/>
+      <c r="L2" s="54"/>
+      <c r="M2" s="54"/>
+      <c r="N2" s="54"/>
+      <c r="O2" s="54"/>
+      <c r="P2" s="54"/>
+      <c r="Q2" s="54"/>
+      <c r="R2" s="54"/>
+      <c r="S2" s="54"/>
+      <c r="T2" s="54"/>
+      <c r="U2" s="54"/>
+      <c r="V2" s="54"/>
+      <c r="W2" s="54"/>
+      <c r="X2" s="54"/>
+      <c r="Y2" s="54"/>
+      <c r="Z2" s="54"/>
+      <c r="AA2" s="54"/>
+      <c r="AB2" s="54"/>
+      <c r="AC2" s="54"/>
+      <c r="AD2" s="54"/>
+      <c r="AE2" s="54"/>
+      <c r="AF2" s="54"/>
+      <c r="AG2" s="54"/>
+      <c r="AH2" s="54"/>
+      <c r="AI2" s="54"/>
+      <c r="AJ2" s="54"/>
+      <c r="AK2" s="54"/>
+      <c r="AL2" s="54"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
@@ -1083,53 +1083,53 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="39" t="s">
+      <c r="D3" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
-      <c r="M3" s="39"/>
-      <c r="N3" s="39"/>
-      <c r="O3" s="39"/>
-      <c r="P3" s="39"/>
-      <c r="Q3" s="39"/>
-      <c r="R3" s="39"/>
-      <c r="S3" s="39"/>
-      <c r="T3" s="39"/>
-      <c r="U3" s="39"/>
-      <c r="V3" s="39"/>
-      <c r="W3" s="39"/>
-      <c r="X3" s="39"/>
-      <c r="Y3" s="39"/>
-      <c r="Z3" s="39"/>
-      <c r="AA3" s="39"/>
-      <c r="AB3" s="39"/>
-      <c r="AC3" s="39"/>
-      <c r="AD3" s="39"/>
-      <c r="AE3" s="39"/>
-      <c r="AF3" s="39"/>
-      <c r="AG3" s="39"/>
-      <c r="AH3" s="39"/>
-      <c r="AI3" s="39"/>
-      <c r="AJ3" s="39"/>
-      <c r="AK3" s="39"/>
-      <c r="AL3" s="39"/>
-      <c r="AM3" s="40"/>
+      <c r="E3" s="58"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="58"/>
+      <c r="H3" s="58"/>
+      <c r="I3" s="58"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="58"/>
+      <c r="L3" s="58"/>
+      <c r="M3" s="58"/>
+      <c r="N3" s="58"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="58"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="58"/>
+      <c r="S3" s="58"/>
+      <c r="T3" s="58"/>
+      <c r="U3" s="58"/>
+      <c r="V3" s="58"/>
+      <c r="W3" s="58"/>
+      <c r="X3" s="58"/>
+      <c r="Y3" s="58"/>
+      <c r="Z3" s="58"/>
+      <c r="AA3" s="58"/>
+      <c r="AB3" s="58"/>
+      <c r="AC3" s="58"/>
+      <c r="AD3" s="58"/>
+      <c r="AE3" s="58"/>
+      <c r="AF3" s="58"/>
+      <c r="AG3" s="58"/>
+      <c r="AH3" s="58"/>
+      <c r="AI3" s="58"/>
+      <c r="AJ3" s="58"/>
+      <c r="AK3" s="58"/>
+      <c r="AL3" s="58"/>
+      <c r="AM3" s="59"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
@@ -1137,49 +1137,49 @@
       <c r="AR3" s="1"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="37"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43" t="s">
+      <c r="A4" s="53"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="43"/>
-      <c r="F4" s="43"/>
-      <c r="G4" s="43"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43"/>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43" t="s">
+      <c r="E4" s="57"/>
+      <c r="F4" s="57"/>
+      <c r="G4" s="57"/>
+      <c r="H4" s="57"/>
+      <c r="I4" s="57"/>
+      <c r="J4" s="57"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
+      <c r="M4" s="57"/>
+      <c r="N4" s="57"/>
+      <c r="O4" s="57"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
+      <c r="R4" s="57"/>
+      <c r="S4" s="57" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="43"/>
-      <c r="Y4" s="43"/>
-      <c r="Z4" s="43"/>
-      <c r="AA4" s="43"/>
-      <c r="AB4" s="43"/>
-      <c r="AC4" s="43"/>
-      <c r="AD4" s="43"/>
-      <c r="AE4" s="43"/>
-      <c r="AF4" s="43"/>
-      <c r="AG4" s="43"/>
-      <c r="AH4" s="43"/>
-      <c r="AI4" s="43"/>
-      <c r="AJ4" s="43"/>
-      <c r="AK4" s="43"/>
-      <c r="AL4" s="43"/>
-      <c r="AM4" s="44"/>
+      <c r="T4" s="57"/>
+      <c r="U4" s="57"/>
+      <c r="V4" s="57"/>
+      <c r="W4" s="57"/>
+      <c r="X4" s="57"/>
+      <c r="Y4" s="57"/>
+      <c r="Z4" s="57"/>
+      <c r="AA4" s="57"/>
+      <c r="AB4" s="57"/>
+      <c r="AC4" s="57"/>
+      <c r="AD4" s="57"/>
+      <c r="AE4" s="57"/>
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="57"/>
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="57"/>
+      <c r="AJ4" s="57"/>
+      <c r="AK4" s="57"/>
+      <c r="AL4" s="57"/>
+      <c r="AM4" s="60"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
@@ -1187,9 +1187,9 @@
       <c r="AR4" s="1"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="37"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
       <c r="D5" s="34">
         <v>17</v>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="AH28" s="16"/>
       <c r="AI28" s="20"/>
       <c r="AJ28" s="20"/>
-      <c r="AK28" s="16"/>
+      <c r="AK28" s="22"/>
       <c r="AL28" s="16"/>
       <c r="AM28" s="17"/>
       <c r="AN28" s="1"/>
@@ -2648,7 +2648,7 @@
       <c r="AI31" s="29"/>
       <c r="AJ31" s="29"/>
       <c r="AK31" s="29"/>
-      <c r="AL31" s="60"/>
+      <c r="AL31" s="36"/>
       <c r="AM31" s="30"/>
       <c r="AN31" s="1"/>
       <c r="AO31" s="1"/>
@@ -2706,168 +2706,168 @@
       <c r="B33" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="45" t="s">
+      <c r="D33" s="37" t="s">
         <v>40</v>
       </c>
-      <c r="E33" s="46"/>
-      <c r="F33" s="46"/>
-      <c r="G33" s="46"/>
-      <c r="H33" s="46"/>
-      <c r="I33" s="46"/>
-      <c r="J33" s="46"/>
-      <c r="K33" s="46"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="46"/>
-      <c r="N33" s="46"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="46"/>
-      <c r="Q33" s="46"/>
-      <c r="R33" s="46"/>
-      <c r="S33" s="46"/>
-      <c r="T33" s="46"/>
-      <c r="U33" s="46"/>
-      <c r="V33" s="46"/>
-      <c r="W33" s="46"/>
-      <c r="X33" s="46"/>
-      <c r="Y33" s="46"/>
-      <c r="Z33" s="46"/>
-      <c r="AA33" s="46"/>
-      <c r="AB33" s="46"/>
-      <c r="AC33" s="46"/>
-      <c r="AD33" s="46"/>
-      <c r="AE33" s="46"/>
-      <c r="AF33" s="46"/>
-      <c r="AG33" s="46"/>
-      <c r="AH33" s="46"/>
-      <c r="AI33" s="46"/>
-      <c r="AJ33" s="46"/>
-      <c r="AK33" s="46"/>
-      <c r="AL33" s="47"/>
+      <c r="E33" s="38"/>
+      <c r="F33" s="38"/>
+      <c r="G33" s="38"/>
+      <c r="H33" s="38"/>
+      <c r="I33" s="38"/>
+      <c r="J33" s="38"/>
+      <c r="K33" s="38"/>
+      <c r="L33" s="38"/>
+      <c r="M33" s="38"/>
+      <c r="N33" s="38"/>
+      <c r="O33" s="38"/>
+      <c r="P33" s="38"/>
+      <c r="Q33" s="38"/>
+      <c r="R33" s="38"/>
+      <c r="S33" s="38"/>
+      <c r="T33" s="38"/>
+      <c r="U33" s="38"/>
+      <c r="V33" s="38"/>
+      <c r="W33" s="38"/>
+      <c r="X33" s="38"/>
+      <c r="Y33" s="38"/>
+      <c r="Z33" s="38"/>
+      <c r="AA33" s="38"/>
+      <c r="AB33" s="38"/>
+      <c r="AC33" s="38"/>
+      <c r="AD33" s="38"/>
+      <c r="AE33" s="38"/>
+      <c r="AF33" s="38"/>
+      <c r="AG33" s="38"/>
+      <c r="AH33" s="38"/>
+      <c r="AI33" s="38"/>
+      <c r="AJ33" s="38"/>
+      <c r="AK33" s="38"/>
+      <c r="AL33" s="39"/>
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="D34" s="48" t="s">
+      <c r="D34" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E34" s="49"/>
-      <c r="F34" s="49"/>
-      <c r="G34" s="49"/>
-      <c r="H34" s="49"/>
-      <c r="I34" s="49"/>
-      <c r="J34" s="49"/>
-      <c r="K34" s="49"/>
-      <c r="L34" s="49"/>
-      <c r="M34" s="49"/>
-      <c r="N34" s="49"/>
-      <c r="O34" s="49"/>
-      <c r="P34" s="49"/>
-      <c r="Q34" s="49"/>
-      <c r="R34" s="49"/>
-      <c r="S34" s="49"/>
-      <c r="T34" s="49"/>
-      <c r="U34" s="49"/>
-      <c r="V34" s="49"/>
-      <c r="W34" s="49"/>
-      <c r="X34" s="49"/>
-      <c r="Y34" s="49"/>
-      <c r="Z34" s="49"/>
-      <c r="AA34" s="49"/>
-      <c r="AB34" s="49"/>
-      <c r="AC34" s="49"/>
-      <c r="AD34" s="49"/>
-      <c r="AE34" s="49"/>
-      <c r="AF34" s="49"/>
-      <c r="AG34" s="49"/>
-      <c r="AH34" s="49"/>
-      <c r="AI34" s="49"/>
-      <c r="AJ34" s="49"/>
-      <c r="AK34" s="49"/>
-      <c r="AL34" s="50"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="41"/>
+      <c r="G34" s="41"/>
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="41"/>
+      <c r="K34" s="41"/>
+      <c r="L34" s="41"/>
+      <c r="M34" s="41"/>
+      <c r="N34" s="41"/>
+      <c r="O34" s="41"/>
+      <c r="P34" s="41"/>
+      <c r="Q34" s="41"/>
+      <c r="R34" s="41"/>
+      <c r="S34" s="41"/>
+      <c r="T34" s="41"/>
+      <c r="U34" s="41"/>
+      <c r="V34" s="41"/>
+      <c r="W34" s="41"/>
+      <c r="X34" s="41"/>
+      <c r="Y34" s="41"/>
+      <c r="Z34" s="41"/>
+      <c r="AA34" s="41"/>
+      <c r="AB34" s="41"/>
+      <c r="AC34" s="41"/>
+      <c r="AD34" s="41"/>
+      <c r="AE34" s="41"/>
+      <c r="AF34" s="41"/>
+      <c r="AG34" s="41"/>
+      <c r="AH34" s="41"/>
+      <c r="AI34" s="41"/>
+      <c r="AJ34" s="41"/>
+      <c r="AK34" s="41"/>
+      <c r="AL34" s="42"/>
     </row>
     <row r="35" spans="1:44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" t="s">
         <v>33</v>
       </c>
-      <c r="D35" s="51"/>
-      <c r="E35" s="52"/>
-      <c r="F35" s="52"/>
-      <c r="G35" s="52"/>
-      <c r="H35" s="52"/>
-      <c r="I35" s="52"/>
-      <c r="J35" s="52"/>
-      <c r="K35" s="52"/>
-      <c r="L35" s="52"/>
-      <c r="M35" s="52"/>
-      <c r="N35" s="52"/>
-      <c r="O35" s="52"/>
-      <c r="P35" s="52"/>
-      <c r="Q35" s="52"/>
-      <c r="R35" s="52"/>
-      <c r="S35" s="52"/>
-      <c r="T35" s="52"/>
-      <c r="U35" s="52"/>
-      <c r="V35" s="52"/>
-      <c r="W35" s="52"/>
-      <c r="X35" s="52"/>
-      <c r="Y35" s="52"/>
-      <c r="Z35" s="52"/>
-      <c r="AA35" s="52"/>
-      <c r="AB35" s="52"/>
-      <c r="AC35" s="52"/>
-      <c r="AD35" s="52"/>
-      <c r="AE35" s="52"/>
-      <c r="AF35" s="52"/>
-      <c r="AG35" s="52"/>
-      <c r="AH35" s="52"/>
-      <c r="AI35" s="52"/>
-      <c r="AJ35" s="52"/>
-      <c r="AK35" s="52"/>
-      <c r="AL35" s="53"/>
+      <c r="D35" s="43"/>
+      <c r="E35" s="44"/>
+      <c r="F35" s="44"/>
+      <c r="G35" s="44"/>
+      <c r="H35" s="44"/>
+      <c r="I35" s="44"/>
+      <c r="J35" s="44"/>
+      <c r="K35" s="44"/>
+      <c r="L35" s="44"/>
+      <c r="M35" s="44"/>
+      <c r="N35" s="44"/>
+      <c r="O35" s="44"/>
+      <c r="P35" s="44"/>
+      <c r="Q35" s="44"/>
+      <c r="R35" s="44"/>
+      <c r="S35" s="44"/>
+      <c r="T35" s="44"/>
+      <c r="U35" s="44"/>
+      <c r="V35" s="44"/>
+      <c r="W35" s="44"/>
+      <c r="X35" s="44"/>
+      <c r="Y35" s="44"/>
+      <c r="Z35" s="44"/>
+      <c r="AA35" s="44"/>
+      <c r="AB35" s="44"/>
+      <c r="AC35" s="44"/>
+      <c r="AD35" s="44"/>
+      <c r="AE35" s="44"/>
+      <c r="AF35" s="44"/>
+      <c r="AG35" s="44"/>
+      <c r="AH35" s="44"/>
+      <c r="AI35" s="44"/>
+      <c r="AJ35" s="44"/>
+      <c r="AK35" s="44"/>
+      <c r="AL35" s="45"/>
     </row>
     <row r="36" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D36" s="54"/>
-      <c r="E36" s="55"/>
-      <c r="F36" s="55"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="55"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="55"/>
-      <c r="N36" s="55"/>
-      <c r="O36" s="55"/>
-      <c r="P36" s="55"/>
-      <c r="Q36" s="55"/>
-      <c r="R36" s="55"/>
-      <c r="S36" s="55"/>
-      <c r="T36" s="55"/>
-      <c r="U36" s="55"/>
-      <c r="V36" s="55"/>
-      <c r="W36" s="55"/>
-      <c r="X36" s="55"/>
-      <c r="Y36" s="55"/>
-      <c r="Z36" s="55"/>
-      <c r="AA36" s="55"/>
-      <c r="AB36" s="55"/>
-      <c r="AC36" s="55"/>
-      <c r="AD36" s="55"/>
-      <c r="AE36" s="55"/>
-      <c r="AF36" s="55"/>
-      <c r="AG36" s="55"/>
-      <c r="AH36" s="55"/>
-      <c r="AI36" s="55"/>
-      <c r="AJ36" s="55"/>
-      <c r="AK36" s="55"/>
-      <c r="AL36" s="56"/>
+      <c r="D36" s="46"/>
+      <c r="E36" s="47"/>
+      <c r="F36" s="47"/>
+      <c r="G36" s="47"/>
+      <c r="H36" s="47"/>
+      <c r="I36" s="47"/>
+      <c r="J36" s="47"/>
+      <c r="K36" s="47"/>
+      <c r="L36" s="47"/>
+      <c r="M36" s="47"/>
+      <c r="N36" s="47"/>
+      <c r="O36" s="47"/>
+      <c r="P36" s="47"/>
+      <c r="Q36" s="47"/>
+      <c r="R36" s="47"/>
+      <c r="S36" s="47"/>
+      <c r="T36" s="47"/>
+      <c r="U36" s="47"/>
+      <c r="V36" s="47"/>
+      <c r="W36" s="47"/>
+      <c r="X36" s="47"/>
+      <c r="Y36" s="47"/>
+      <c r="Z36" s="47"/>
+      <c r="AA36" s="47"/>
+      <c r="AB36" s="47"/>
+      <c r="AC36" s="47"/>
+      <c r="AD36" s="47"/>
+      <c r="AE36" s="47"/>
+      <c r="AF36" s="47"/>
+      <c r="AG36" s="47"/>
+      <c r="AH36" s="47"/>
+      <c r="AI36" s="47"/>
+      <c r="AJ36" s="47"/>
+      <c r="AK36" s="47"/>
+      <c r="AL36" s="48"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
       <c r="AP36" s="1"/>
@@ -2879,41 +2879,41 @@
       <c r="B37" s="32" t="s">
         <v>39</v>
       </c>
-      <c r="D37" s="57"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
-      <c r="J37" s="58"/>
-      <c r="K37" s="58"/>
-      <c r="L37" s="58"/>
-      <c r="M37" s="58"/>
-      <c r="N37" s="58"/>
-      <c r="O37" s="58"/>
-      <c r="P37" s="58"/>
-      <c r="Q37" s="58"/>
-      <c r="R37" s="58"/>
-      <c r="S37" s="58"/>
-      <c r="T37" s="58"/>
-      <c r="U37" s="58"/>
-      <c r="V37" s="58"/>
-      <c r="W37" s="58"/>
-      <c r="X37" s="58"/>
-      <c r="Y37" s="58"/>
-      <c r="Z37" s="58"/>
-      <c r="AA37" s="58"/>
-      <c r="AB37" s="58"/>
-      <c r="AC37" s="58"/>
-      <c r="AD37" s="58"/>
-      <c r="AE37" s="58"/>
-      <c r="AF37" s="58"/>
-      <c r="AG37" s="58"/>
-      <c r="AH37" s="58"/>
-      <c r="AI37" s="58"/>
-      <c r="AJ37" s="58"/>
-      <c r="AK37" s="58"/>
-      <c r="AL37" s="59"/>
+      <c r="D37" s="49"/>
+      <c r="E37" s="50"/>
+      <c r="F37" s="50"/>
+      <c r="G37" s="50"/>
+      <c r="H37" s="50"/>
+      <c r="I37" s="50"/>
+      <c r="J37" s="50"/>
+      <c r="K37" s="50"/>
+      <c r="L37" s="50"/>
+      <c r="M37" s="50"/>
+      <c r="N37" s="50"/>
+      <c r="O37" s="50"/>
+      <c r="P37" s="50"/>
+      <c r="Q37" s="50"/>
+      <c r="R37" s="50"/>
+      <c r="S37" s="50"/>
+      <c r="T37" s="50"/>
+      <c r="U37" s="50"/>
+      <c r="V37" s="50"/>
+      <c r="W37" s="50"/>
+      <c r="X37" s="50"/>
+      <c r="Y37" s="50"/>
+      <c r="Z37" s="50"/>
+      <c r="AA37" s="50"/>
+      <c r="AB37" s="50"/>
+      <c r="AC37" s="50"/>
+      <c r="AD37" s="50"/>
+      <c r="AE37" s="50"/>
+      <c r="AF37" s="50"/>
+      <c r="AG37" s="50"/>
+      <c r="AH37" s="50"/>
+      <c r="AI37" s="50"/>
+      <c r="AJ37" s="50"/>
+      <c r="AK37" s="50"/>
+      <c r="AL37" s="51"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
     </row>
@@ -3406,11 +3406,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="D33:AL33"/>
-    <mergeCell ref="D34:AL34"/>
-    <mergeCell ref="D35:AL35"/>
-    <mergeCell ref="D36:AL36"/>
-    <mergeCell ref="D37:AL37"/>
     <mergeCell ref="A3:A5"/>
     <mergeCell ref="A1:AL2"/>
     <mergeCell ref="B3:B5"/>
@@ -3418,6 +3413,11 @@
     <mergeCell ref="D4:R4"/>
     <mergeCell ref="D3:AM3"/>
     <mergeCell ref="S4:AM4"/>
+    <mergeCell ref="D33:AL33"/>
+    <mergeCell ref="D34:AL34"/>
+    <mergeCell ref="D35:AL35"/>
+    <mergeCell ref="D36:AL36"/>
+    <mergeCell ref="D37:AL37"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Se organizó todo para impresión y preparación
</commit_message>
<xml_diff>
--- a/Gantt.xlsx
+++ b/Gantt.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="42">
   <si>
     <t>Rochín</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Impresión de la portada de la caja</t>
   </si>
   <si>
-    <t>Compra o adquisición de la caja</t>
-  </si>
-  <si>
     <t>Elaboración de Instalador Binario</t>
   </si>
   <si>
@@ -144,9 +141,6 @@
     <t>Diseño del servidor</t>
   </si>
   <si>
-    <t>Se retomó la tarea</t>
-  </si>
-  <si>
     <t>Notas</t>
   </si>
   <si>
@@ -154,6 +148,9 @@
   </si>
   <si>
     <t>Texturizado de objetos</t>
+  </si>
+  <si>
+    <t>Compra o adquisición de la caja y disco</t>
   </si>
 </sst>
 </file>
@@ -198,7 +195,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,12 +250,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFEFC9F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -419,12 +410,23 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.499984740745262"/>
@@ -435,7 +437,7 @@
       <left/>
       <right/>
       <top style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.499984740745262"/>
@@ -445,10 +447,10 @@
     <border>
       <left/>
       <right style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </right>
       <top style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.499984740745262"/>
@@ -457,7 +459,7 @@
     </border>
     <border>
       <left style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
       <top style="thin">
@@ -465,6 +467,32 @@
       </top>
       <bottom style="thin">
         <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.499984740745262"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -474,58 +502,21 @@
       <top style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </right>
       <top style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
       <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color theme="1"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="medium">
-        <color theme="1"/>
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -533,7 +524,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -588,8 +579,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -597,30 +586,27 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
@@ -971,10 +957,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR51"/>
+  <dimension ref="A1:AR50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="AK28" sqref="AK28"/>
+      <selection activeCell="W24" sqref="W24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,46 +975,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
-      <c r="O1" s="54"/>
-      <c r="P1" s="54"/>
-      <c r="Q1" s="54"/>
-      <c r="R1" s="54"/>
-      <c r="S1" s="54"/>
-      <c r="T1" s="54"/>
-      <c r="U1" s="54"/>
-      <c r="V1" s="54"/>
-      <c r="W1" s="54"/>
-      <c r="X1" s="54"/>
-      <c r="Y1" s="54"/>
-      <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AD1" s="54"/>
-      <c r="AE1" s="54"/>
-      <c r="AF1" s="54"/>
-      <c r="AG1" s="54"/>
-      <c r="AH1" s="54"/>
-      <c r="AI1" s="54"/>
-      <c r="AJ1" s="54"/>
-      <c r="AK1" s="54"/>
-      <c r="AL1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="49"/>
+      <c r="V1" s="49"/>
+      <c r="W1" s="49"/>
+      <c r="X1" s="49"/>
+      <c r="Y1" s="49"/>
+      <c r="Z1" s="49"/>
+      <c r="AA1" s="49"/>
+      <c r="AB1" s="49"/>
+      <c r="AC1" s="49"/>
+      <c r="AD1" s="49"/>
+      <c r="AE1" s="49"/>
+      <c r="AF1" s="49"/>
+      <c r="AG1" s="49"/>
+      <c r="AH1" s="49"/>
+      <c r="AI1" s="49"/>
+      <c r="AJ1" s="49"/>
+      <c r="AK1" s="49"/>
+      <c r="AL1" s="49"/>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
@@ -1037,44 +1023,44 @@
       <c r="AR1" s="1"/>
     </row>
     <row r="2" spans="1:44" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="54"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
-      <c r="G2" s="54"/>
-      <c r="H2" s="54"/>
-      <c r="I2" s="54"/>
-      <c r="J2" s="54"/>
-      <c r="K2" s="54"/>
-      <c r="L2" s="54"/>
-      <c r="M2" s="54"/>
-      <c r="N2" s="54"/>
-      <c r="O2" s="54"/>
-      <c r="P2" s="54"/>
-      <c r="Q2" s="54"/>
-      <c r="R2" s="54"/>
-      <c r="S2" s="54"/>
-      <c r="T2" s="54"/>
-      <c r="U2" s="54"/>
-      <c r="V2" s="54"/>
-      <c r="W2" s="54"/>
-      <c r="X2" s="54"/>
-      <c r="Y2" s="54"/>
-      <c r="Z2" s="54"/>
-      <c r="AA2" s="54"/>
-      <c r="AB2" s="54"/>
-      <c r="AC2" s="54"/>
-      <c r="AD2" s="54"/>
-      <c r="AE2" s="54"/>
-      <c r="AF2" s="54"/>
-      <c r="AG2" s="54"/>
-      <c r="AH2" s="54"/>
-      <c r="AI2" s="54"/>
-      <c r="AJ2" s="54"/>
-      <c r="AK2" s="54"/>
-      <c r="AL2" s="54"/>
+      <c r="A2" s="49"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49"/>
       <c r="AM2" s="1"/>
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
@@ -1083,53 +1069,53 @@
       <c r="AR2" s="1"/>
     </row>
     <row r="3" spans="1:44" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="52" t="s">
+      <c r="A3" s="47" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="55" t="s">
+      <c r="B3" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="55" t="s">
+      <c r="C3" s="50" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="53" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58"/>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58"/>
-      <c r="AC3" s="58"/>
-      <c r="AD3" s="58"/>
-      <c r="AE3" s="58"/>
-      <c r="AF3" s="58"/>
-      <c r="AG3" s="58"/>
-      <c r="AH3" s="58"/>
-      <c r="AI3" s="58"/>
-      <c r="AJ3" s="58"/>
-      <c r="AK3" s="58"/>
-      <c r="AL3" s="58"/>
-      <c r="AM3" s="59"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
+      <c r="M3" s="53"/>
+      <c r="N3" s="53"/>
+      <c r="O3" s="53"/>
+      <c r="P3" s="53"/>
+      <c r="Q3" s="53"/>
+      <c r="R3" s="53"/>
+      <c r="S3" s="53"/>
+      <c r="T3" s="53"/>
+      <c r="U3" s="53"/>
+      <c r="V3" s="53"/>
+      <c r="W3" s="53"/>
+      <c r="X3" s="53"/>
+      <c r="Y3" s="53"/>
+      <c r="Z3" s="53"/>
+      <c r="AA3" s="53"/>
+      <c r="AB3" s="53"/>
+      <c r="AC3" s="53"/>
+      <c r="AD3" s="53"/>
+      <c r="AE3" s="53"/>
+      <c r="AF3" s="53"/>
+      <c r="AG3" s="53"/>
+      <c r="AH3" s="53"/>
+      <c r="AI3" s="53"/>
+      <c r="AJ3" s="53"/>
+      <c r="AK3" s="53"/>
+      <c r="AL3" s="53"/>
+      <c r="AM3" s="54"/>
       <c r="AN3" s="1"/>
       <c r="AO3" s="1"/>
       <c r="AP3" s="1"/>
@@ -1137,49 +1123,49 @@
       <c r="AR3" s="1"/>
     </row>
     <row r="4" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A4" s="53"/>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="57" t="s">
+      <c r="A4" s="48"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="57"/>
-      <c r="F4" s="57"/>
-      <c r="G4" s="57"/>
-      <c r="H4" s="57"/>
-      <c r="I4" s="57"/>
-      <c r="J4" s="57"/>
-      <c r="K4" s="57"/>
-      <c r="L4" s="57"/>
-      <c r="M4" s="57"/>
-      <c r="N4" s="57"/>
-      <c r="O4" s="57"/>
-      <c r="P4" s="57"/>
-      <c r="Q4" s="57"/>
-      <c r="R4" s="57"/>
-      <c r="S4" s="57" t="s">
+      <c r="E4" s="52"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="52"/>
+      <c r="H4" s="52"/>
+      <c r="I4" s="52"/>
+      <c r="J4" s="52"/>
+      <c r="K4" s="52"/>
+      <c r="L4" s="52"/>
+      <c r="M4" s="52"/>
+      <c r="N4" s="52"/>
+      <c r="O4" s="52"/>
+      <c r="P4" s="52"/>
+      <c r="Q4" s="52"/>
+      <c r="R4" s="52"/>
+      <c r="S4" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="T4" s="57"/>
-      <c r="U4" s="57"/>
-      <c r="V4" s="57"/>
-      <c r="W4" s="57"/>
-      <c r="X4" s="57"/>
-      <c r="Y4" s="57"/>
-      <c r="Z4" s="57"/>
-      <c r="AA4" s="57"/>
-      <c r="AB4" s="57"/>
-      <c r="AC4" s="57"/>
-      <c r="AD4" s="57"/>
-      <c r="AE4" s="57"/>
-      <c r="AF4" s="57"/>
-      <c r="AG4" s="57"/>
-      <c r="AH4" s="57"/>
-      <c r="AI4" s="57"/>
-      <c r="AJ4" s="57"/>
-      <c r="AK4" s="57"/>
-      <c r="AL4" s="57"/>
-      <c r="AM4" s="60"/>
+      <c r="T4" s="52"/>
+      <c r="U4" s="52"/>
+      <c r="V4" s="52"/>
+      <c r="W4" s="52"/>
+      <c r="X4" s="52"/>
+      <c r="Y4" s="52"/>
+      <c r="Z4" s="52"/>
+      <c r="AA4" s="52"/>
+      <c r="AB4" s="52"/>
+      <c r="AC4" s="52"/>
+      <c r="AD4" s="52"/>
+      <c r="AE4" s="52"/>
+      <c r="AF4" s="52"/>
+      <c r="AG4" s="52"/>
+      <c r="AH4" s="52"/>
+      <c r="AI4" s="52"/>
+      <c r="AJ4" s="52"/>
+      <c r="AK4" s="52"/>
+      <c r="AL4" s="52"/>
+      <c r="AM4" s="55"/>
       <c r="AN4" s="1"/>
       <c r="AO4" s="1"/>
       <c r="AP4" s="1"/>
@@ -1187,115 +1173,115 @@
       <c r="AR4" s="1"/>
     </row>
     <row r="5" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="A5" s="53"/>
-      <c r="B5" s="56"/>
-      <c r="C5" s="56"/>
-      <c r="D5" s="34">
+      <c r="A5" s="48"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="51"/>
+      <c r="D5" s="32">
         <v>17</v>
       </c>
-      <c r="E5" s="34">
+      <c r="E5" s="32">
         <v>18</v>
       </c>
-      <c r="F5" s="34">
+      <c r="F5" s="32">
         <v>19</v>
       </c>
-      <c r="G5" s="34">
+      <c r="G5" s="32">
         <v>20</v>
       </c>
-      <c r="H5" s="34">
+      <c r="H5" s="32">
         <v>21</v>
       </c>
-      <c r="I5" s="34">
+      <c r="I5" s="32">
         <v>22</v>
       </c>
-      <c r="J5" s="34">
+      <c r="J5" s="32">
         <v>23</v>
       </c>
-      <c r="K5" s="34">
+      <c r="K5" s="32">
         <v>24</v>
       </c>
-      <c r="L5" s="34">
+      <c r="L5" s="32">
         <v>25</v>
       </c>
-      <c r="M5" s="34">
+      <c r="M5" s="32">
         <v>26</v>
       </c>
-      <c r="N5" s="34">
+      <c r="N5" s="32">
         <v>27</v>
       </c>
-      <c r="O5" s="34">
+      <c r="O5" s="32">
         <v>28</v>
       </c>
-      <c r="P5" s="34">
+      <c r="P5" s="32">
         <v>29</v>
       </c>
-      <c r="Q5" s="34">
+      <c r="Q5" s="32">
         <v>30</v>
       </c>
-      <c r="R5" s="34">
+      <c r="R5" s="32">
         <v>31</v>
       </c>
-      <c r="S5" s="34">
+      <c r="S5" s="32">
         <v>1</v>
       </c>
-      <c r="T5" s="34">
+      <c r="T5" s="32">
         <v>2</v>
       </c>
-      <c r="U5" s="34">
+      <c r="U5" s="32">
         <v>3</v>
       </c>
-      <c r="V5" s="34">
+      <c r="V5" s="32">
         <v>4</v>
       </c>
-      <c r="W5" s="34">
+      <c r="W5" s="32">
         <v>5</v>
       </c>
-      <c r="X5" s="34">
+      <c r="X5" s="32">
         <v>6</v>
       </c>
-      <c r="Y5" s="34">
+      <c r="Y5" s="32">
         <v>7</v>
       </c>
-      <c r="Z5" s="34">
+      <c r="Z5" s="32">
         <v>8</v>
       </c>
-      <c r="AA5" s="34">
+      <c r="AA5" s="32">
         <v>9</v>
       </c>
-      <c r="AB5" s="34">
+      <c r="AB5" s="32">
         <v>10</v>
       </c>
-      <c r="AC5" s="34">
+      <c r="AC5" s="32">
         <v>11</v>
       </c>
-      <c r="AD5" s="34">
+      <c r="AD5" s="32">
         <v>12</v>
       </c>
-      <c r="AE5" s="34">
+      <c r="AE5" s="32">
         <v>13</v>
       </c>
-      <c r="AF5" s="34">
+      <c r="AF5" s="32">
         <v>14</v>
       </c>
-      <c r="AG5" s="34">
+      <c r="AG5" s="32">
         <v>15</v>
       </c>
-      <c r="AH5" s="34">
+      <c r="AH5" s="32">
         <v>16</v>
       </c>
-      <c r="AI5" s="34">
+      <c r="AI5" s="32">
         <v>17</v>
       </c>
-      <c r="AJ5" s="34">
+      <c r="AJ5" s="32">
         <v>18</v>
       </c>
-      <c r="AK5" s="34">
+      <c r="AK5" s="32">
         <v>19</v>
       </c>
-      <c r="AL5" s="34">
+      <c r="AL5" s="32">
         <v>20</v>
       </c>
-      <c r="AM5" s="35">
+      <c r="AM5" s="33">
         <v>21</v>
       </c>
       <c r="AN5" s="1"/>
@@ -1520,7 +1506,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="14"/>
@@ -1572,7 +1558,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="14"/>
@@ -1780,7 +1766,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="16"/>
       <c r="E15" s="16"/>
@@ -1832,7 +1818,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D16" s="16"/>
       <c r="E16" s="16"/>
@@ -2196,7 +2182,7 @@
         <v>0</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
@@ -2300,7 +2286,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="D25" s="16"/>
       <c r="E25" s="16"/>
@@ -2456,7 +2442,7 @@
         <v>0</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D28" s="16"/>
       <c r="E28" s="16"/>
@@ -2508,7 +2494,7 @@
         <v>0</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="16"/>
       <c r="E29" s="16"/>
@@ -2648,7 +2634,7 @@
       <c r="AI31" s="29"/>
       <c r="AJ31" s="29"/>
       <c r="AK31" s="29"/>
-      <c r="AL31" s="36"/>
+      <c r="AL31" s="34"/>
       <c r="AM31" s="30"/>
       <c r="AN31" s="1"/>
       <c r="AO31" s="1"/>
@@ -2704,216 +2690,178 @@
     <row r="33" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A33" s="6"/>
       <c r="B33" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="D33" s="37" t="s">
-        <v>40</v>
-      </c>
-      <c r="E33" s="38"/>
-      <c r="F33" s="38"/>
-      <c r="G33" s="38"/>
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
-      <c r="J33" s="38"/>
-      <c r="K33" s="38"/>
-      <c r="L33" s="38"/>
-      <c r="M33" s="38"/>
-      <c r="N33" s="38"/>
-      <c r="O33" s="38"/>
-      <c r="P33" s="38"/>
-      <c r="Q33" s="38"/>
-      <c r="R33" s="38"/>
-      <c r="S33" s="38"/>
-      <c r="T33" s="38"/>
-      <c r="U33" s="38"/>
-      <c r="V33" s="38"/>
-      <c r="W33" s="38"/>
-      <c r="X33" s="38"/>
-      <c r="Y33" s="38"/>
-      <c r="Z33" s="38"/>
-      <c r="AA33" s="38"/>
-      <c r="AB33" s="38"/>
-      <c r="AC33" s="38"/>
-      <c r="AD33" s="38"/>
-      <c r="AE33" s="38"/>
-      <c r="AF33" s="38"/>
-      <c r="AG33" s="38"/>
-      <c r="AH33" s="38"/>
-      <c r="AI33" s="38"/>
-      <c r="AJ33" s="38"/>
-      <c r="AK33" s="38"/>
-      <c r="AL33" s="39"/>
+        <v>30</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="36"/>
+      <c r="F33" s="36"/>
+      <c r="G33" s="36"/>
+      <c r="H33" s="36"/>
+      <c r="I33" s="36"/>
+      <c r="J33" s="36"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="36"/>
+      <c r="O33" s="36"/>
+      <c r="P33" s="36"/>
+      <c r="Q33" s="36"/>
+      <c r="R33" s="36"/>
+      <c r="S33" s="36"/>
+      <c r="T33" s="36"/>
+      <c r="U33" s="36"/>
+      <c r="V33" s="36"/>
+      <c r="W33" s="36"/>
+      <c r="X33" s="36"/>
+      <c r="Y33" s="36"/>
+      <c r="Z33" s="36"/>
+      <c r="AA33" s="36"/>
+      <c r="AB33" s="36"/>
+      <c r="AC33" s="36"/>
+      <c r="AD33" s="36"/>
+      <c r="AE33" s="36"/>
+      <c r="AF33" s="36"/>
+      <c r="AG33" s="36"/>
+      <c r="AH33" s="36"/>
+      <c r="AI33" s="36"/>
+      <c r="AJ33" s="36"/>
+      <c r="AK33" s="36"/>
+      <c r="AL33" s="37"/>
     </row>
     <row r="34" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="D34" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E34" s="41"/>
-      <c r="F34" s="41"/>
-      <c r="G34" s="41"/>
-      <c r="H34" s="41"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="41"/>
-      <c r="L34" s="41"/>
-      <c r="M34" s="41"/>
-      <c r="N34" s="41"/>
-      <c r="O34" s="41"/>
-      <c r="P34" s="41"/>
-      <c r="Q34" s="41"/>
-      <c r="R34" s="41"/>
-      <c r="S34" s="41"/>
-      <c r="T34" s="41"/>
-      <c r="U34" s="41"/>
-      <c r="V34" s="41"/>
-      <c r="W34" s="41"/>
-      <c r="X34" s="41"/>
-      <c r="Y34" s="41"/>
-      <c r="Z34" s="41"/>
-      <c r="AA34" s="41"/>
-      <c r="AB34" s="41"/>
-      <c r="AC34" s="41"/>
-      <c r="AD34" s="41"/>
-      <c r="AE34" s="41"/>
-      <c r="AF34" s="41"/>
-      <c r="AG34" s="41"/>
-      <c r="AH34" s="41"/>
-      <c r="AI34" s="41"/>
-      <c r="AJ34" s="41"/>
-      <c r="AK34" s="41"/>
-      <c r="AL34" s="42"/>
+        <v>31</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="39"/>
+      <c r="H34" s="39"/>
+      <c r="I34" s="39"/>
+      <c r="J34" s="39"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="39"/>
+      <c r="N34" s="39"/>
+      <c r="O34" s="39"/>
+      <c r="P34" s="39"/>
+      <c r="Q34" s="39"/>
+      <c r="R34" s="39"/>
+      <c r="S34" s="39"/>
+      <c r="T34" s="39"/>
+      <c r="U34" s="39"/>
+      <c r="V34" s="39"/>
+      <c r="W34" s="39"/>
+      <c r="X34" s="39"/>
+      <c r="Y34" s="39"/>
+      <c r="Z34" s="39"/>
+      <c r="AA34" s="39"/>
+      <c r="AB34" s="39"/>
+      <c r="AC34" s="39"/>
+      <c r="AD34" s="39"/>
+      <c r="AE34" s="39"/>
+      <c r="AF34" s="39"/>
+      <c r="AG34" s="39"/>
+      <c r="AH34" s="39"/>
+      <c r="AI34" s="39"/>
+      <c r="AJ34" s="39"/>
+      <c r="AK34" s="39"/>
+      <c r="AL34" s="40"/>
     </row>
     <row r="35" spans="1:44" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="8"/>
       <c r="B35" t="s">
-        <v>33</v>
-      </c>
-      <c r="D35" s="43"/>
-      <c r="E35" s="44"/>
-      <c r="F35" s="44"/>
-      <c r="G35" s="44"/>
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
-      <c r="K35" s="44"/>
-      <c r="L35" s="44"/>
-      <c r="M35" s="44"/>
-      <c r="N35" s="44"/>
-      <c r="O35" s="44"/>
-      <c r="P35" s="44"/>
-      <c r="Q35" s="44"/>
-      <c r="R35" s="44"/>
-      <c r="S35" s="44"/>
-      <c r="T35" s="44"/>
-      <c r="U35" s="44"/>
-      <c r="V35" s="44"/>
-      <c r="W35" s="44"/>
-      <c r="X35" s="44"/>
-      <c r="Y35" s="44"/>
-      <c r="Z35" s="44"/>
-      <c r="AA35" s="44"/>
-      <c r="AB35" s="44"/>
-      <c r="AC35" s="44"/>
-      <c r="AD35" s="44"/>
-      <c r="AE35" s="44"/>
-      <c r="AF35" s="44"/>
-      <c r="AG35" s="44"/>
-      <c r="AH35" s="44"/>
-      <c r="AI35" s="44"/>
-      <c r="AJ35" s="44"/>
-      <c r="AK35" s="44"/>
-      <c r="AL35" s="45"/>
-    </row>
-    <row r="36" spans="1:44" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="D35" s="41"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="42"/>
+      <c r="G35" s="42"/>
+      <c r="H35" s="42"/>
+      <c r="I35" s="42"/>
+      <c r="J35" s="42"/>
+      <c r="K35" s="42"/>
+      <c r="L35" s="42"/>
+      <c r="M35" s="42"/>
+      <c r="N35" s="42"/>
+      <c r="O35" s="42"/>
+      <c r="P35" s="42"/>
+      <c r="Q35" s="42"/>
+      <c r="R35" s="42"/>
+      <c r="S35" s="42"/>
+      <c r="T35" s="42"/>
+      <c r="U35" s="42"/>
+      <c r="V35" s="42"/>
+      <c r="W35" s="42"/>
+      <c r="X35" s="42"/>
+      <c r="Y35" s="42"/>
+      <c r="Z35" s="42"/>
+      <c r="AA35" s="42"/>
+      <c r="AB35" s="42"/>
+      <c r="AC35" s="42"/>
+      <c r="AD35" s="42"/>
+      <c r="AE35" s="42"/>
+      <c r="AF35" s="42"/>
+      <c r="AG35" s="42"/>
+      <c r="AH35" s="42"/>
+      <c r="AI35" s="42"/>
+      <c r="AJ35" s="42"/>
+      <c r="AK35" s="42"/>
+      <c r="AL35" s="43"/>
+    </row>
+    <row r="36" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="9"/>
       <c r="B36" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D36" s="46"/>
-      <c r="E36" s="47"/>
-      <c r="F36" s="47"/>
-      <c r="G36" s="47"/>
-      <c r="H36" s="47"/>
-      <c r="I36" s="47"/>
-      <c r="J36" s="47"/>
-      <c r="K36" s="47"/>
-      <c r="L36" s="47"/>
-      <c r="M36" s="47"/>
-      <c r="N36" s="47"/>
-      <c r="O36" s="47"/>
-      <c r="P36" s="47"/>
-      <c r="Q36" s="47"/>
-      <c r="R36" s="47"/>
-      <c r="S36" s="47"/>
-      <c r="T36" s="47"/>
-      <c r="U36" s="47"/>
-      <c r="V36" s="47"/>
-      <c r="W36" s="47"/>
-      <c r="X36" s="47"/>
-      <c r="Y36" s="47"/>
-      <c r="Z36" s="47"/>
-      <c r="AA36" s="47"/>
-      <c r="AB36" s="47"/>
-      <c r="AC36" s="47"/>
-      <c r="AD36" s="47"/>
-      <c r="AE36" s="47"/>
-      <c r="AF36" s="47"/>
-      <c r="AG36" s="47"/>
-      <c r="AH36" s="47"/>
-      <c r="AI36" s="47"/>
-      <c r="AJ36" s="47"/>
-      <c r="AK36" s="47"/>
-      <c r="AL36" s="48"/>
+        <v>33</v>
+      </c>
+      <c r="D36" s="44"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="45"/>
+      <c r="G36" s="45"/>
+      <c r="H36" s="45"/>
+      <c r="I36" s="45"/>
+      <c r="J36" s="45"/>
+      <c r="K36" s="45"/>
+      <c r="L36" s="45"/>
+      <c r="M36" s="45"/>
+      <c r="N36" s="45"/>
+      <c r="O36" s="45"/>
+      <c r="P36" s="45"/>
+      <c r="Q36" s="45"/>
+      <c r="R36" s="45"/>
+      <c r="S36" s="45"/>
+      <c r="T36" s="45"/>
+      <c r="U36" s="45"/>
+      <c r="V36" s="45"/>
+      <c r="W36" s="45"/>
+      <c r="X36" s="45"/>
+      <c r="Y36" s="45"/>
+      <c r="Z36" s="45"/>
+      <c r="AA36" s="45"/>
+      <c r="AB36" s="45"/>
+      <c r="AC36" s="45"/>
+      <c r="AD36" s="45"/>
+      <c r="AE36" s="45"/>
+      <c r="AF36" s="45"/>
+      <c r="AG36" s="45"/>
+      <c r="AH36" s="45"/>
+      <c r="AI36" s="45"/>
+      <c r="AJ36" s="45"/>
+      <c r="AK36" s="45"/>
+      <c r="AL36" s="46"/>
       <c r="AN36" s="1"/>
       <c r="AO36" s="1"/>
       <c r="AP36" s="1"/>
       <c r="AQ36" s="1"/>
       <c r="AR36" s="1"/>
     </row>
-    <row r="37" spans="1:44" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="33"/>
-      <c r="B37" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D37" s="49"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="50"/>
-      <c r="J37" s="50"/>
-      <c r="K37" s="50"/>
-      <c r="L37" s="50"/>
-      <c r="M37" s="50"/>
-      <c r="N37" s="50"/>
-      <c r="O37" s="50"/>
-      <c r="P37" s="50"/>
-      <c r="Q37" s="50"/>
-      <c r="R37" s="50"/>
-      <c r="S37" s="50"/>
-      <c r="T37" s="50"/>
-      <c r="U37" s="50"/>
-      <c r="V37" s="50"/>
-      <c r="W37" s="50"/>
-      <c r="X37" s="50"/>
-      <c r="Y37" s="50"/>
-      <c r="Z37" s="50"/>
-      <c r="AA37" s="50"/>
-      <c r="AB37" s="50"/>
-      <c r="AC37" s="50"/>
-      <c r="AD37" s="50"/>
-      <c r="AE37" s="50"/>
-      <c r="AF37" s="50"/>
-      <c r="AG37" s="50"/>
-      <c r="AH37" s="50"/>
-      <c r="AI37" s="50"/>
-      <c r="AJ37" s="50"/>
-      <c r="AK37" s="50"/>
-      <c r="AL37" s="51"/>
+    <row r="37" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="B37" s="2"/>
       <c r="AN37" s="1"/>
       <c r="AO37" s="1"/>
     </row>
@@ -2924,11 +2872,48 @@
     </row>
     <row r="39" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B39" s="2"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="4"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="O39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="4"/>
+      <c r="R39" s="4"/>
+      <c r="S39" s="4"/>
+      <c r="T39" s="4"/>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="4"/>
+      <c r="X39" s="4"/>
+      <c r="Y39" s="4"/>
+      <c r="Z39" s="4"/>
+      <c r="AA39" s="4"/>
+      <c r="AB39" s="4"/>
+      <c r="AC39" s="4"/>
+      <c r="AD39" s="4"/>
+      <c r="AE39" s="4"/>
+      <c r="AF39" s="4"/>
+      <c r="AG39" s="4"/>
+      <c r="AH39" s="4"/>
+      <c r="AI39" s="4"/>
+      <c r="AJ39" s="4"/>
+      <c r="AK39" s="4"/>
+      <c r="AL39" s="4"/>
+      <c r="AM39" s="4"/>
       <c r="AN39" s="1"/>
       <c r="AO39" s="1"/>
     </row>
     <row r="40" spans="1:44" x14ac:dyDescent="0.25">
-      <c r="B40" s="2"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="4"/>
       <c r="H40" s="4"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
@@ -2961,8 +2946,6 @@
       <c r="AK40" s="4"/>
       <c r="AL40" s="4"/>
       <c r="AM40" s="4"/>
-      <c r="AN40" s="1"/>
-      <c r="AO40" s="1"/>
     </row>
     <row r="41" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B41" s="3"/>
@@ -3364,49 +3347,8 @@
       <c r="AL50" s="4"/>
       <c r="AM50" s="4"/>
     </row>
-    <row r="51" spans="2:39" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
-      <c r="F51" s="4"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
-      <c r="J51" s="4"/>
-      <c r="K51" s="4"/>
-      <c r="L51" s="4"/>
-      <c r="M51" s="4"/>
-      <c r="N51" s="4"/>
-      <c r="O51" s="4"/>
-      <c r="P51" s="4"/>
-      <c r="Q51" s="4"/>
-      <c r="R51" s="4"/>
-      <c r="S51" s="4"/>
-      <c r="T51" s="4"/>
-      <c r="U51" s="4"/>
-      <c r="V51" s="4"/>
-      <c r="W51" s="4"/>
-      <c r="X51" s="4"/>
-      <c r="Y51" s="4"/>
-      <c r="Z51" s="4"/>
-      <c r="AA51" s="4"/>
-      <c r="AB51" s="4"/>
-      <c r="AC51" s="4"/>
-      <c r="AD51" s="4"/>
-      <c r="AE51" s="4"/>
-      <c r="AF51" s="4"/>
-      <c r="AG51" s="4"/>
-      <c r="AH51" s="4"/>
-      <c r="AI51" s="4"/>
-      <c r="AJ51" s="4"/>
-      <c r="AK51" s="4"/>
-      <c r="AL51" s="4"/>
-      <c r="AM51" s="4"/>
-    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="A3:A5"/>
+  <mergeCells count="11">
     <mergeCell ref="A1:AL2"/>
     <mergeCell ref="B3:B5"/>
     <mergeCell ref="C3:C5"/>
@@ -3417,7 +3359,7 @@
     <mergeCell ref="D34:AL34"/>
     <mergeCell ref="D35:AL35"/>
     <mergeCell ref="D36:AL36"/>
-    <mergeCell ref="D37:AL37"/>
+    <mergeCell ref="A3:A5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>